<commit_message>
Models fitting and graphed
</commit_message>
<xml_diff>
--- a/model_outputs/tyre_ranking.xlsx
+++ b/model_outputs/tyre_ranking.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,13 +10,13 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE3334B-244A-4467-BBB3-8BDA03662D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="89" uniqueCount="44">
   <si>
     <t>'SA_at_FY_max'</t>
   </si>
@@ -166,13 +166,16 @@
   </si>
   <si>
     <t>Selection Matrix Weightings</t>
+  </si>
+  <si>
+    <t>12_Hoosier_20.5x7-13_R20_8Rim.tir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,7 +200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -205,13 +208,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -230,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -381,7 +386,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -405,9 +410,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -431,7 +436,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -466,7 +471,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -484,7 +489,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -509,7 +514,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -545,33 +550,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.4140625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="40.1640625" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="14.9140625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="14.4140625" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="22.4140625" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="16.4140625" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="14.75" customWidth="true"/>
+    <col min="8" max="8" width="12.6640625" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="13" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="8.58203125" bestFit="true" customWidth="true"/>
+    <col min="11" max="11" width="14.58203125" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="14.5" bestFit="true" customWidth="true"/>
+    <col min="13" max="13" width="14.33203125" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="16.5" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="22.58203125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -618,7 +623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -665,7 +670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -709,48 +714,54 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
-        <v>1221.5396764871136</v>
-      </c>
-      <c r="F4">
-        <v>1039.5260389762489</v>
-      </c>
-      <c r="G4">
-        <v>14322.622536600144</v>
-      </c>
-      <c r="H4">
-        <v>12376.420038468304</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C4" s="0">
+        <v>-11.363636363636363</v>
+      </c>
+      <c r="D4" s="0">
+        <v>1378.5647730407597</v>
+      </c>
+      <c r="E4" s="0">
+        <v>-11.363636363636363</v>
+      </c>
+      <c r="F4" s="0">
+        <v>1152.3653094664892</v>
+      </c>
+      <c r="G4" s="0">
+        <v>19143.469473247831</v>
+      </c>
+      <c r="H4" s="0">
+        <v>16469.351270755647</v>
+      </c>
+      <c r="I4" s="0">
+        <v>1</v>
+      </c>
+      <c r="J4" s="0">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -797,17 +808,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -854,7 +865,7 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -901,7 +912,7 @@
         <v>6.2121212121212119</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -948,7 +959,7 @@
         <v>4.3939393939393936</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>10.757575757575756</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1042,7 +1053,54 @@
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13">
+      <c r="A13" s="0">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="0">
+        <v>-5.9090909090909092</v>
+      </c>
+      <c r="D13" s="0">
+        <v>1446.814738053685</v>
+      </c>
+      <c r="E13" s="0">
+        <v>-5.6060606060606055</v>
+      </c>
+      <c r="F13" s="0">
+        <v>1213.769009670656</v>
+      </c>
+      <c r="G13" s="0">
+        <v>36968.755564889514</v>
+      </c>
+      <c r="H13" s="0">
+        <v>31950.493206296178</v>
+      </c>
+      <c r="I13" s="0">
+        <v>1</v>
+      </c>
+      <c r="J13" s="0">
+        <v>1</v>
+      </c>
+      <c r="K13" s="0">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0">
+        <v>1286.6649923608313</v>
+      </c>
+      <c r="M13" s="0">
+        <v>7.7272727272727275</v>
+      </c>
+      <c r="N13" s="0">
+        <v>1073.7162945574842</v>
+      </c>
+      <c r="O13" s="0">
+        <v>8.0303030303030294</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1089,7 +1147,7 @@
         <v>8.6363636363636367</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1136,7 +1194,7 @@
         <v>6.8181818181818175</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1183,7 +1241,7 @@
         <v>5.6060606060606055</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1230,7 +1288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1277,7 +1335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1324,7 +1382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1371,7 +1429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1418,7 +1476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1465,7 +1523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1512,7 +1570,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1556,7 +1614,7 @@
         <v>1085.2972477264514</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1603,7 +1661,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1650,7 +1708,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1697,7 +1755,7 @@
         <v>11.666666666666664</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1750,16 +1808,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Added and minorly reformatted calspan summary tables
</commit_message>
<xml_diff>
--- a/model_outputs/tyre_ranking.xlsx
+++ b/model_outputs/tyre_ranking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\GitHub\cmt_tyre_toolbox_new\model_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAE9C96-2855-456C-BF01-E91FBDDC616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D6249-79CA-4FBF-AC15-29D0E5A6AB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,9 +204,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +543,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,7 +572,7 @@
       <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
@@ -620,7 +619,7 @@
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>-9.545454545454545</v>
       </c>
       <c r="D2">
@@ -667,7 +666,7 @@
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>-11.363636363636363</v>
       </c>
       <c r="D3">
@@ -714,7 +713,7 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>-11.363636363636363</v>
       </c>
       <c r="D4">
@@ -761,7 +760,7 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>-12.878787878787877</v>
       </c>
       <c r="D5">
@@ -808,7 +807,7 @@
       <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>-8.6363636363636367</v>
       </c>
       <c r="D6">
@@ -855,7 +854,7 @@
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>-9.545454545454545</v>
       </c>
       <c r="D7">
@@ -896,7 +895,7 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>-7.7272727272727275</v>
       </c>
       <c r="D8">
@@ -943,7 +942,7 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>-8.0303030303030294</v>
       </c>
       <c r="D9">
@@ -990,7 +989,7 @@
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>-4.3939393939393936</v>
       </c>
       <c r="D10">
@@ -1037,7 +1036,7 @@
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>-4.3939393939393936</v>
       </c>
       <c r="D11">
@@ -1084,7 +1083,7 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>-7.1212121212121202</v>
       </c>
       <c r="D12">

</xml_diff>

<commit_message>
Code clean up and new functionality?
</commit_message>
<xml_diff>
--- a/model_outputs/tyre_ranking.xlsx
+++ b/model_outputs/tyre_ranking.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_tyre_toolbox_new\model_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E4EFD2-6F64-4DBF-8751-84C689B82D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95643D7A-563A-4AA6-A65E-FFAD31A2B08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" fullCalcOnLoad="true"/>
+  <fileRecoveryPr repairLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="141" uniqueCount="70">
   <si>
     <t>'SA_at_FY_max'</t>
   </si>
@@ -242,11 +243,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -383,57 +384,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +455,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -603,7 +606,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -627,9 +630,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -653,7 +656,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -688,7 +691,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -706,7 +709,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -731,7 +734,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -767,32 +770,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
-  <dimension ref="A1:O28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
+  <dimension ref="A1:DJ28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="40.875" customWidth="true"/>
+    <col min="3" max="3" width="14.5" customWidth="true"/>
+    <col min="4" max="4" width="15" customWidth="true"/>
+    <col min="5" max="5" width="22.875" customWidth="true"/>
+    <col min="6" max="6" width="17" customWidth="true"/>
+    <col min="7" max="7" width="15.375" customWidth="true"/>
+    <col min="8" max="8" width="13.125" customWidth="true"/>
+    <col min="9" max="9" width="13.375" customWidth="true"/>
+    <col min="10" max="10" width="8.75" customWidth="true"/>
+    <col min="11" max="11" width="14.625" customWidth="true"/>
+    <col min="12" max="12" width="15" customWidth="true"/>
+    <col min="13" max="13" width="14.75" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="17" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="23.125" customWidth="true"/>
+    <col min="16" max="16" width="12.25" customWidth="true"/>
+    <col min="17" max="17" width="12.25" customWidth="true"/>
+    <col min="18" max="18" width="12.25" customWidth="true"/>
+    <col min="19" max="19" width="12.25" customWidth="true"/>
+    <col min="20" max="20" width="12.25" customWidth="true"/>
+    <col min="21" max="21" width="12.25" customWidth="true"/>
+    <col min="22" max="22" width="12.25" customWidth="true"/>
+    <col min="23" max="23" width="11.25" customWidth="true"/>
+    <col min="24" max="24" width="12.25" customWidth="true"/>
+    <col min="25" max="25" width="11.625" customWidth="true"/>
+    <col min="26" max="26" width="11.625" customWidth="true"/>
+    <col min="27" max="27" width="11.625" customWidth="true"/>
+    <col min="28" max="28" width="11.625" customWidth="true"/>
+    <col min="29" max="29" width="11.625" customWidth="true"/>
+    <col min="30" max="30" width="11.625" customWidth="true"/>
+    <col min="31" max="31" width="11.625" customWidth="true"/>
+    <col min="32" max="32" width="11.625" customWidth="true"/>
+    <col min="33" max="33" width="11.625" customWidth="true"/>
+    <col min="34" max="34" width="10.625" customWidth="true"/>
+    <col min="35" max="35" width="11.625" customWidth="true"/>
+    <col min="36" max="36" width="11.625" customWidth="true"/>
+    <col min="37" max="37" width="10.625" customWidth="true"/>
+    <col min="38" max="38" width="9.625" customWidth="true"/>
+    <col min="39" max="39" width="11.625" customWidth="true"/>
+    <col min="40" max="40" width="11.625" customWidth="true"/>
+    <col min="41" max="41" width="11.625" customWidth="true"/>
+    <col min="42" max="42" width="11.625" customWidth="true"/>
+    <col min="43" max="43" width="11.625" customWidth="true"/>
+    <col min="44" max="44" width="11.625" customWidth="true"/>
+    <col min="45" max="45" width="11.625" customWidth="true"/>
+    <col min="46" max="46" width="11.625" customWidth="true"/>
+    <col min="47" max="47" width="11.625" customWidth="true"/>
+    <col min="48" max="48" width="11.625" customWidth="true"/>
+    <col min="49" max="49" width="11.625" customWidth="true"/>
+    <col min="50" max="50" width="11.625" customWidth="true"/>
+    <col min="51" max="51" width="11.625" customWidth="true"/>
+    <col min="52" max="52" width="11.625" customWidth="true"/>
+    <col min="53" max="53" width="11.625" customWidth="true"/>
+    <col min="54" max="54" width="11.625" customWidth="true"/>
+    <col min="55" max="55" width="11.625" customWidth="true"/>
+    <col min="56" max="56" width="10.625" customWidth="true"/>
+    <col min="57" max="57" width="11.625" customWidth="true"/>
+    <col min="58" max="58" width="11.625" customWidth="true"/>
+    <col min="59" max="59" width="11.625" customWidth="true"/>
+    <col min="60" max="60" width="11.625" customWidth="true"/>
+    <col min="61" max="61" width="11.625" customWidth="true"/>
+    <col min="62" max="62" width="11.625" customWidth="true"/>
+    <col min="63" max="63" width="11.625" customWidth="true"/>
+    <col min="64" max="64" width="11.625" customWidth="true"/>
+    <col min="65" max="65" width="11.625" customWidth="true"/>
+    <col min="66" max="66" width="11.625" customWidth="true"/>
+    <col min="67" max="67" width="11.625" customWidth="true"/>
+    <col min="68" max="68" width="11.625" customWidth="true"/>
+    <col min="69" max="69" width="11.625" customWidth="true"/>
+    <col min="70" max="70" width="11.625" customWidth="true"/>
+    <col min="71" max="71" width="11.625" customWidth="true"/>
+    <col min="72" max="72" width="11.625" customWidth="true"/>
+    <col min="73" max="73" width="11.625" customWidth="true"/>
+    <col min="74" max="74" width="11.625" customWidth="true"/>
+    <col min="75" max="75" width="11.625" customWidth="true"/>
+    <col min="76" max="76" width="11.625" customWidth="true"/>
+    <col min="77" max="77" width="11.625" customWidth="true"/>
+    <col min="78" max="78" width="10.625" customWidth="true"/>
+    <col min="79" max="79" width="11.625" customWidth="true"/>
+    <col min="80" max="80" width="11.625" customWidth="true"/>
+    <col min="81" max="81" width="11.625" customWidth="true"/>
+    <col min="82" max="82" width="11.625" customWidth="true"/>
+    <col min="83" max="83" width="11.625" customWidth="true"/>
+    <col min="84" max="84" width="11.625" customWidth="true"/>
+    <col min="85" max="85" width="11.625" customWidth="true"/>
+    <col min="86" max="86" width="11.625" customWidth="true"/>
+    <col min="87" max="87" width="11.625" customWidth="true"/>
+    <col min="88" max="88" width="11.625" customWidth="true"/>
+    <col min="89" max="89" width="11.625" customWidth="true"/>
+    <col min="90" max="90" width="11.625" customWidth="true"/>
+    <col min="91" max="91" width="10.625" customWidth="true"/>
+    <col min="92" max="92" width="11.625" customWidth="true"/>
+    <col min="93" max="93" width="11.625" customWidth="true"/>
+    <col min="94" max="94" width="11.625" customWidth="true"/>
+    <col min="95" max="95" width="11.625" customWidth="true"/>
+    <col min="96" max="96" width="11.625" customWidth="true"/>
+    <col min="97" max="97" width="11.625" customWidth="true"/>
+    <col min="98" max="98" width="11.625" customWidth="true"/>
+    <col min="99" max="99" width="12.25" customWidth="true"/>
+    <col min="100" max="100" width="12.25" customWidth="true"/>
+    <col min="101" max="101" width="12.25" customWidth="true"/>
+    <col min="102" max="102" width="12.25" customWidth="true"/>
+    <col min="103" max="103" width="12.25" customWidth="true"/>
+    <col min="104" max="104" width="11.25" customWidth="true"/>
+    <col min="105" max="105" width="12.25" customWidth="true"/>
+    <col min="106" max="106" width="10.25" customWidth="true"/>
+    <col min="107" max="107" width="10.625" customWidth="true"/>
+    <col min="108" max="108" width="2.125" customWidth="true"/>
+    <col min="109" max="109" width="2.125" customWidth="true"/>
+    <col min="110" max="110" width="2.125" customWidth="true"/>
+    <col min="111" max="111" width="11.625" customWidth="true"/>
+    <col min="112" max="112" width="9.140625"/>
+    <col min="113" max="113" width="11.625" customWidth="true"/>
+    <col min="114" max="114" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -839,7 +942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -886,7 +989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -933,7 +1036,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -980,7 +1083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1027,7 +1130,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1074,48 +1177,343 @@
         <v>11.363636363636363</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>-9.545454545454545</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>1488.1734889619829</v>
       </c>
-      <c r="E7">
-        <v>-9.2424242424242422</v>
-      </c>
-      <c r="F7">
-        <v>1248.4949159330297</v>
-      </c>
-      <c r="G7">
+      <c r="E7" s="0">
+        <v>-9.545454545454545</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1428.7543587969342</v>
+      </c>
+      <c r="G7" s="0">
         <v>23057.299498565211</v>
       </c>
-      <c r="H7">
-        <v>19881.696810483798</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
+      <c r="H7" s="0">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0">
+        <v>1</v>
+      </c>
+      <c r="K7" s="0">
         <v>1251.1047378194853</v>
       </c>
-      <c r="N7">
-        <v>1044.8106880542593</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L7" s="0"/>
+      <c r="M7" s="0">
+        <v>1199.7725693945349</v>
+      </c>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0">
+        <v>-613.05747106264187</v>
+      </c>
+      <c r="P7" s="0">
+        <v>-586.86562986268325</v>
+      </c>
+      <c r="Q7" s="0">
+        <v>-555.36988010621099</v>
+      </c>
+      <c r="R7" s="0">
+        <v>-517.82000547540838</v>
+      </c>
+      <c r="S7" s="0">
+        <v>-473.36078157677622</v>
+      </c>
+      <c r="T7" s="0">
+        <v>-421.01713982212186</v>
+      </c>
+      <c r="U7" s="0">
+        <v>-359.67734635648799</v>
+      </c>
+      <c r="V7" s="0">
+        <v>-288.07400173447297</v>
+      </c>
+      <c r="W7" s="0">
+        <v>-204.76268200950426</v>
+      </c>
+      <c r="X7" s="0">
+        <v>-108.0980763831508</v>
+      </c>
+      <c r="Y7" s="0">
+        <v>3.792460308245782</v>
+      </c>
+      <c r="Z7" s="0">
+        <v>133.03791774346317</v>
+      </c>
+      <c r="AA7" s="0">
+        <v>282.05501820760145</v>
+      </c>
+      <c r="AB7" s="0">
+        <v>453.58155556052361</v>
+      </c>
+      <c r="AC7" s="0">
+        <v>650.71090643684636</v>
+      </c>
+      <c r="AD7" s="0">
+        <v>876.92643730238399</v>
+      </c>
+      <c r="AE7" s="0">
+        <v>1136.1338414274937</v>
+      </c>
+      <c r="AF7" s="0">
+        <v>1432.6885041341261</v>
+      </c>
+      <c r="AG7" s="0">
+        <v>1771.413751946847</v>
+      </c>
+      <c r="AH7" s="0">
+        <v>2157.6042296027836</v>
+      </c>
+      <c r="AI7" s="0">
+        <v>2597.0066166254178</v>
+      </c>
+      <c r="AJ7" s="0">
+        <v>3095.7674215164402</v>
+      </c>
+      <c r="AK7" s="0">
+        <v>3660.3347204813149</v>
+      </c>
+      <c r="AL7" s="0">
+        <v>4297.2975998351294</v>
+      </c>
+      <c r="AM7" s="0">
+        <v>5013.1440691547041</v>
+      </c>
+      <c r="AN7" s="0">
+        <v>5813.9159766118473</v>
+      </c>
+      <c r="AO7" s="0">
+        <v>6704.7390181288074</v>
+      </c>
+      <c r="AP7" s="0">
+        <v>7689.2088218431491</v>
+      </c>
+      <c r="AQ7" s="0">
+        <v>8768.6223608158525</v>
+      </c>
+      <c r="AR7" s="0">
+        <v>9941.0600231576555</v>
+      </c>
+      <c r="AS7" s="0">
+        <v>11200.349886716876</v>
+      </c>
+      <c r="AT7" s="0">
+        <v>12534.983434842145</v>
+      </c>
+      <c r="AU7" s="0">
+        <v>13927.09996489036</v>
+      </c>
+      <c r="AV7" s="0">
+        <v>15351.709786815538</v>
+      </c>
+      <c r="AW7" s="0">
+        <v>16776.372430645155</v>
+      </c>
+      <c r="AX7" s="0">
+        <v>18161.567467442852</v>
+      </c>
+      <c r="AY7" s="0">
+        <v>19461.970225823039</v>
+      </c>
+      <c r="AZ7" s="0">
+        <v>20628.753410666093</v>
+      </c>
+      <c r="BA7" s="0">
+        <v>21612.872448233506</v>
+      </c>
+      <c r="BB7" s="0">
+        <v>22369.075714987877</v>
+      </c>
+      <c r="BC7" s="0">
+        <v>22860.158570280597</v>
+      </c>
+      <c r="BD7" s="0">
+        <v>23057.299498565211</v>
+      </c>
+      <c r="BE7" s="0">
+        <v>22923.748407237079</v>
+      </c>
+      <c r="BF7" s="0">
+        <v>22437.494706857433</v>
+      </c>
+      <c r="BG7" s="0">
+        <v>21623.984440493772</v>
+      </c>
+      <c r="BH7" s="0">
+        <v>20538.522812032177</v>
+      </c>
+      <c r="BI7" s="0">
+        <v>19248.691528025865</v>
+      </c>
+      <c r="BJ7" s="0">
+        <v>17825.642016051799</v>
+      </c>
+      <c r="BK7" s="0">
+        <v>16336.567356744574</v>
+      </c>
+      <c r="BL7" s="0">
+        <v>14839.402990256525</v>
+      </c>
+      <c r="BM7" s="0">
+        <v>13380.049289633778</v>
+      </c>
+      <c r="BN7" s="0">
+        <v>11991.796078617735</v>
+      </c>
+      <c r="BO7" s="0">
+        <v>10696.311425008143</v>
+      </c>
+      <c r="BP7" s="0">
+        <v>9505.5080136035558</v>
+      </c>
+      <c r="BQ7" s="0">
+        <v>8423.7193127405917</v>
+      </c>
+      <c r="BR7" s="0">
+        <v>7449.7999836696163</v>
+      </c>
+      <c r="BS7" s="0">
+        <v>6578.9386967403379</v>
+      </c>
+      <c r="BT7" s="0">
+        <v>5804.1030634318749</v>
+      </c>
+      <c r="BU7" s="0">
+        <v>5117.1197772985715</v>
+      </c>
+      <c r="BV7" s="0">
+        <v>4509.4365041203127</v>
+      </c>
+      <c r="BW7" s="0">
+        <v>3972.6280264108909</v>
+      </c>
+      <c r="BX7" s="0">
+        <v>3498.7089541061769</v>
+      </c>
+      <c r="BY7" s="0">
+        <v>3080.30724414837</v>
+      </c>
+      <c r="BZ7" s="0">
+        <v>2710.7420397867977</v>
+      </c>
+      <c r="CA7" s="0">
+        <v>2384.0387932531298</v>
+      </c>
+      <c r="CB7" s="0">
+        <v>2094.905560894078</v>
+      </c>
+      <c r="CC7" s="0">
+        <v>1838.6871381081394</v>
+      </c>
+      <c r="CD7" s="0">
+        <v>1611.3082506389146</v>
+      </c>
+      <c r="CE7" s="0">
+        <v>1409.2130649902579</v>
+      </c>
+      <c r="CF7" s="0">
+        <v>1229.3055047596529</v>
+      </c>
+      <c r="CG7" s="0">
+        <v>1068.8929668449532</v>
+      </c>
+      <c r="CH7" s="0">
+        <v>925.63477772662782</v>
+      </c>
+      <c r="CI7" s="0">
+        <v>797.49592585473749</v>
+      </c>
+      <c r="CJ7" s="0">
+        <v>682.70611061710179</v>
+      </c>
+      <c r="CK7" s="0">
+        <v>579.72385983203128</v>
+      </c>
+      <c r="CL7" s="0">
+        <v>487.20531475168951</v>
+      </c>
+      <c r="CM7" s="0">
+        <v>403.97721497913955</v>
+      </c>
+      <c r="CN7" s="0">
+        <v>329.01360224340488</v>
+      </c>
+      <c r="CO7" s="0">
+        <v>261.41577959383721</v>
+      </c>
+      <c r="CP7" s="0">
+        <v>200.39509693933607</v>
+      </c>
+      <c r="CQ7" s="0">
+        <v>145.25817588716407</v>
+      </c>
+      <c r="CR7" s="0">
+        <v>95.394230946490381</v>
+      </c>
+      <c r="CS7" s="0">
+        <v>50.264187077637473</v>
+      </c>
+      <c r="CT7" s="0">
+        <v>9.3913335039392152</v>
+      </c>
+      <c r="CU7" s="0">
+        <v>-27.646710186902439</v>
+      </c>
+      <c r="CV7" s="0">
+        <v>-61.224907605849857</v>
+      </c>
+      <c r="CW7" s="0">
+        <v>-91.676762743225325</v>
+      </c>
+      <c r="CX7" s="0">
+        <v>-119.29946047376022</v>
+      </c>
+      <c r="CY7" s="0">
+        <v>-144.3583092509582</v>
+      </c>
+      <c r="CZ7" s="0">
+        <v>-167.09058703389817</v>
+      </c>
+      <c r="DA7" s="0">
+        <v>-187.70887630870376</v>
+      </c>
+      <c r="DB7" s="0">
+        <v>-197.51465001559578</v>
+      </c>
+      <c r="DC7" s="0">
+        <v>23057.299498565211</v>
+      </c>
+      <c r="DD7" s="0">
+        <v>1</v>
+      </c>
+      <c r="DE7" s="0">
+        <v>1</v>
+      </c>
+      <c r="DF7" s="0">
+        <v>1</v>
+      </c>
+      <c r="DG7" s="0">
+        <v>1251.1047378194853</v>
+      </c>
+      <c r="DH7" s="0"/>
+      <c r="DI7" s="0">
+        <v>1199.7725693945349</v>
+      </c>
+      <c r="DJ7" s="0"/>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1162,7 +1560,7 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1209,7 +1607,7 @@
         <v>6.2121212121212119</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1256,7 +1654,7 @@
         <v>4.3939393939393936</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1303,7 +1701,7 @@
         <v>10.757575757575756</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1350,7 +1748,7 @@
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1397,7 +1795,7 @@
         <v>8.0303030303030294</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1444,7 +1842,7 @@
         <v>8.6363636363636367</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1491,7 +1889,7 @@
         <v>6.8181818181818175</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1538,7 +1936,7 @@
         <v>5.6060606060606055</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1585,7 +1983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1632,7 +2030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1679,7 +2077,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1726,7 +2124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1773,7 +2171,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1820,7 +2218,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1867,7 +2265,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1911,7 +2309,7 @@
         <v>1085.2972477264514</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1958,7 +2356,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2005,7 +2403,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2052,7 +2450,7 @@
         <v>11.666666666666664</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2105,110 +2503,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9038B9-1403-4B22-9A5D-BC5487C92A60}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
+  <dimension ref="B1:AA66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="true"/>
+    <col min="3" max="3" width="21.42578125" customWidth="true"/>
+    <col min="4" max="5" width="18.42578125" customWidth="true"/>
+    <col min="6" max="6" width="13.7109375" bestFit="true" customWidth="true"/>
+    <col min="7" max="10" width="13.7109375" customWidth="true"/>
+    <col min="11" max="11" width="11.5703125" customWidth="true"/>
+    <col min="21" max="21" width="37.85546875" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="e">
-        <f ca="1">xlookup(A2,Sheet3!B40:B66, Sheet3!R40:R66)</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
-  <dimension ref="B1:AA66"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="37.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="F1" s="16" t="s">
         <v>65</v>
       </c>
@@ -2216,12 +2529,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:27" ht="39" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" ht="39" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>Sheet1!$B$1</f>
         <v>'tyre'</v>
@@ -2272,7 +2585,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>51</v>
       </c>
@@ -2319,7 +2632,7 @@
         <v>1.4750000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
@@ -2362,7 +2675,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>Sheet1!B2</f>
         <v>01_Hoosier_16x7.5-10_R20_7Rim.tir</v>
@@ -2379,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="19">
-        <f>C7-D7</f>
+        <f t="shared" ref="F7:F33" si="0">C7-D7</f>
         <v>229.86324473627474</v>
       </c>
       <c r="G7" s="9">
@@ -2405,7 +2718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>Sheet1!B3</f>
         <v>02_Hoosier_16x7.5-10_R20_8Rim.tir</v>
@@ -2422,7 +2735,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="19">
-        <f>C8-D8</f>
+        <f t="shared" si="0"/>
         <v>229.82545093101089</v>
       </c>
       <c r="G8" s="9">
@@ -2437,7 +2750,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="19">
-        <f t="shared" ref="J8:J33" si="0">G8-H8</f>
+        <f t="shared" ref="J8:J33" si="1">G8-H8</f>
         <v>0</v>
       </c>
       <c r="L8" s="9">
@@ -2451,7 +2764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>Sheet1!B4</f>
         <v>03_Hoosier_16x6.0-10_R20_6Rim.tir</v>
@@ -2468,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="19">
-        <f>C9-D9</f>
+        <f t="shared" si="0"/>
         <v>226.19946357427057</v>
       </c>
       <c r="G9" s="9">
@@ -2483,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L9" s="9">
@@ -2506,7 +2819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f>Sheet1!B5</f>
         <v>04_Hoosier_16x6.0-10_R20_7Rim.tir</v>
@@ -2523,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="19">
-        <f>C10-D10</f>
+        <f t="shared" si="0"/>
         <v>220.06734385699883</v>
       </c>
       <c r="G10" s="9">
@@ -2538,7 +2851,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L10" s="9">
@@ -2549,7 +2862,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>Sheet1!B6</f>
         <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
@@ -2566,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="19">
-        <f>C11-D11</f>
+        <f t="shared" si="0"/>
         <v>230.92713867535713</v>
       </c>
       <c r="G11" s="9">
@@ -2581,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>214.45739238377587</v>
       </c>
       <c r="L11" s="9">
@@ -2592,7 +2905,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>Sheet1!B7</f>
         <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
@@ -2609,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="19">
-        <f>C12-D12</f>
+        <f t="shared" si="0"/>
         <v>239.67857302895322</v>
       </c>
       <c r="G12" s="9">
@@ -2624,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>206.29404976522596</v>
       </c>
       <c r="L12" s="9">
@@ -2635,7 +2948,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>Sheet1!B8</f>
         <v>07_Goodyear_18.0x6.5-10_D0571_6Rim.tir</v>
@@ -2652,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="19">
-        <f>C13-D13</f>
+        <f t="shared" si="0"/>
         <v>240.89047967612419</v>
       </c>
       <c r="G13" s="9">
@@ -2667,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>217.60167076401535</v>
       </c>
       <c r="L13" s="9">
@@ -2678,7 +2991,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>Sheet1!B9</f>
         <v>08_Goodyear_18.0x6.5-10_D0571_7Rim.tir</v>
@@ -2695,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="19">
-        <f>C14-D14</f>
+        <f t="shared" si="0"/>
         <v>241.60241346468774</v>
       </c>
       <c r="G14" s="9">
@@ -2710,7 +3023,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>222.10243990067238</v>
       </c>
       <c r="L14" s="9">
@@ -2721,7 +3034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>Sheet1!B10</f>
         <v>09_MRF_18x6-10_ZTD1_6Rim.tir</v>
@@ -2738,7 +3051,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="19">
-        <f>C15-D15</f>
+        <f t="shared" si="0"/>
         <v>186.1672738863017</v>
       </c>
       <c r="G15" s="9">
@@ -2753,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>177.45800110760638</v>
       </c>
       <c r="L15" s="9">
@@ -2764,7 +3077,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>Sheet1!B11</f>
         <v>10_MRF_18x6-10_ZTD1_7Rim.tir</v>
@@ -2781,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="19">
-        <f>C16-D16</f>
+        <f t="shared" si="0"/>
         <v>182.62619939434944</v>
       </c>
       <c r="G16" s="9">
@@ -2796,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>176.73268346237103</v>
       </c>
       <c r="L16" s="9">
@@ -2807,7 +3120,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>Sheet1!B12</f>
         <v>11_Hoosier_20.5x7-13_R20_7Rim.tir</v>
@@ -2824,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="19">
-        <f>C17-D17</f>
+        <f t="shared" si="0"/>
         <v>238.85482152454551</v>
       </c>
       <c r="G17" s="9">
@@ -2839,7 +3152,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>217.90108416787575</v>
       </c>
       <c r="L17" s="9">
@@ -2850,7 +3163,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>Sheet1!B13</f>
         <v>12_Hoosier_20.5x7-13_R20_8Rim.tir</v>
@@ -2867,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="19">
-        <f>C18-D18</f>
+        <f t="shared" si="0"/>
         <v>233.04572838302897</v>
       </c>
       <c r="G18" s="9">
@@ -2882,7 +3195,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>212.94869780334716</v>
       </c>
       <c r="L18" s="9">
@@ -2890,7 +3203,7 @@
         <v>36968.755564889514</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>Sheet1!B14</f>
         <v>13_Goodyear_20.0x7-13_D2704_7Rim.tir</v>
@@ -2907,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="19">
-        <f>C19-D19</f>
+        <f t="shared" si="0"/>
         <v>266.82908962217743</v>
       </c>
       <c r="G19" s="9">
@@ -2922,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>206.0819946487876</v>
       </c>
       <c r="L19" s="9">
@@ -2930,7 +3243,7 @@
         <v>29240.85832208081</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>Sheet1!B15</f>
         <v>14_Goodyear_20.0x7-13_D2704_8Rim.tir</v>
@@ -2947,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="19">
-        <f>C20-D20</f>
+        <f t="shared" si="0"/>
         <v>235.60532053892439</v>
       </c>
       <c r="G20" s="9">
@@ -2962,7 +3275,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>215.71322098213636</v>
       </c>
       <c r="L20" s="9">
@@ -2970,7 +3283,7 @@
         <v>27410.226980274612</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>Sheet1!B16</f>
         <v>15_Continental_205x470R-13_FS43329_7Rim.tir</v>
@@ -2987,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="19">
-        <f>C21-D21</f>
+        <f t="shared" si="0"/>
         <v>249.22030828404741</v>
       </c>
       <c r="G21" s="9">
@@ -3002,7 +3315,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>220.06776510944474</v>
       </c>
       <c r="L21" s="9">
@@ -3010,7 +3323,7 @@
         <v>30766.058316327431</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>Sheet1!B17</f>
         <v>16_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
@@ -3027,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="19">
-        <f>C22-D22</f>
+        <f t="shared" si="0"/>
         <v>212.2841030489576</v>
       </c>
       <c r="G22" s="9">
@@ -3042,7 +3355,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L22" s="9">
@@ -3050,7 +3363,7 @@
         <v>19958.48151666945</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>Sheet1!B18</f>
         <v>17_Hoosier_16.0x6.0-10_LCO_7Rim.tir</v>
@@ -3067,7 +3380,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="19">
-        <f>C23-D23</f>
+        <f t="shared" si="0"/>
         <v>215.09981394738361</v>
       </c>
       <c r="G23" s="9">
@@ -3082,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L23" s="9">
@@ -3090,7 +3403,7 @@
         <v>21253.399390250874</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>Sheet1!B19</f>
         <v>18_Hoosier_16.0x7.5-10_LCO_8Rim.tir</v>
@@ -3107,7 +3420,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="19">
-        <f>C24-D24</f>
+        <f t="shared" si="0"/>
         <v>216.15602670815997</v>
       </c>
       <c r="G24" s="9">
@@ -3122,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L24" s="9">
@@ -3130,7 +3443,7 @@
         <v>20065.804846484891</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>Sheet1!B20</f>
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
@@ -3147,7 +3460,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="19">
-        <f>C25-D25</f>
+        <f t="shared" si="0"/>
         <v>222.38518555231872</v>
       </c>
       <c r="G25" s="9">
@@ -3162,7 +3475,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L25" s="9">
@@ -3170,7 +3483,7 @@
         <v>20428.69287290483</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>Sheet1!B21</f>
         <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
@@ -3187,7 +3500,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="19">
-        <f>C26-D26</f>
+        <f t="shared" si="0"/>
         <v>195.2363051985119</v>
       </c>
       <c r="G26" s="9">
@@ -3202,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L26" s="9">
@@ -3210,7 +3523,7 @@
         <v>18859.597365099344</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>Sheet1!B22</f>
         <v>21_Avon_7.0x16.0-11_FS_8Rim.tir</v>
@@ -3227,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="19">
-        <f>C27-D27</f>
+        <f t="shared" si="0"/>
         <v>191.11143790584651</v>
       </c>
       <c r="G27" s="9">
@@ -3242,7 +3555,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L27" s="9">
@@ -3250,7 +3563,7 @@
         <v>20378.311960636642</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>Sheet1!B23</f>
         <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
@@ -3267,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="19">
-        <f>C28-D28</f>
+        <f t="shared" si="0"/>
         <v>227.93759011810312</v>
       </c>
       <c r="G28" s="9">
@@ -3282,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>212.53238105396758</v>
       </c>
       <c r="L28" s="9">
@@ -3290,7 +3603,7 @@
         <v>18597.177761836752</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
         <f>Sheet1!B24</f>
         <v>23_Avon_8.2x20.0-14_FS_9Rim.tir</v>
@@ -3307,7 +3620,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="19">
-        <f>C29-D29</f>
+        <f t="shared" si="0"/>
         <v>217.78077610485252</v>
       </c>
       <c r="G29" s="9">
@@ -3322,7 +3635,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>209.53606215492778</v>
       </c>
       <c r="L29" s="9">
@@ -3330,7 +3643,7 @@
         <v>19024.110013201633</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f>Sheet1!B25</f>
         <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
@@ -3347,7 +3660,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="19">
-        <f>C30-D30</f>
+        <f t="shared" si="0"/>
         <v>204.5124674352669</v>
       </c>
       <c r="G30" s="9">
@@ -3362,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>185.96063193242969</v>
       </c>
       <c r="L30" s="9">
@@ -3370,7 +3683,7 @@
         <v>16336.480118847954</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>Sheet1!B26</f>
         <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
@@ -3387,7 +3700,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="19">
-        <f>C31-D31</f>
+        <f t="shared" si="0"/>
         <v>196.8895735740291</v>
       </c>
       <c r="G31" s="9">
@@ -3402,7 +3715,7 @@
         <v>1</v>
       </c>
       <c r="J31" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>199.46627066505903</v>
       </c>
       <c r="L31" s="9">
@@ -3410,7 +3723,7 @@
         <v>16745.947522921681</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>Sheet1!B27</f>
         <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
@@ -3427,7 +3740,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="19">
-        <f>C32-D32</f>
+        <f t="shared" si="0"/>
         <v>188.80458466887842</v>
       </c>
       <c r="G32" s="9">
@@ -3442,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>181.07513686079619</v>
       </c>
       <c r="L32" s="9">
@@ -3450,7 +3763,7 @@
         <v>15324.620447760168</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>Sheet1!B28</f>
         <v>27_Avon_6.2x20.0-14_FS_7Rim.tir</v>
@@ -3467,7 +3780,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="19">
-        <f>C33-D33</f>
+        <f t="shared" si="0"/>
         <v>274.05176123431011</v>
       </c>
       <c r="G33" s="9">
@@ -3482,7 +3795,7 @@
         <v>1</v>
       </c>
       <c r="J33" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>187.24304462794146</v>
       </c>
       <c r="L33" s="9">
@@ -3490,12 +3803,12 @@
         <v>8358.4992902210615</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="36" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:18" ht="39" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="37" ht="39" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>Sheet1!$B$1</f>
         <v>'tyre'</v>
@@ -3546,7 +3859,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="38" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>51</v>
       </c>
@@ -3563,43 +3876,43 @@
         <v>0.15</v>
       </c>
       <c r="G38" s="11">
-        <f t="shared" ref="D38:P38" si="1">G5</f>
+        <f t="shared" ref="G38:P38" si="2">G5</f>
         <v>0.15</v>
       </c>
       <c r="H38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="I38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="K38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="L38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="M38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="N38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="O38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="P38" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="Q38" s="7">
@@ -3607,7 +3920,7 @@
         <v>1.4500000000000002</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="39" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>52</v>
       </c>
@@ -3616,7 +3929,7 @@
         <v>0.1</v>
       </c>
       <c r="D39" s="10">
-        <f t="shared" ref="D39:P39" si="2">D38</f>
+        <f t="shared" ref="D39:P39" si="3">D38</f>
         <v>0.1</v>
       </c>
       <c r="E39" s="10">
@@ -3624,47 +3937,47 @@
         <v>0.1</v>
       </c>
       <c r="F39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="G39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="H39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="I39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
       <c r="K39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="L39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.125</v>
       </c>
       <c r="M39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="N39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="O39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="P39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="Q39" s="2"/>
@@ -3672,7 +3985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="40" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>B7</f>
         <v>01_Hoosier_16x7.5-10_R20_7Rim.tir</v>
@@ -3719,38 +4032,38 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="41" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
-        <f t="shared" ref="B41:B66" si="3">B8</f>
+        <f t="shared" ref="B41:B66" si="4">B8</f>
         <v>02_Hoosier_16x7.5-10_R20_8Rim.tir</v>
       </c>
       <c r="C41" s="18">
-        <f t="shared" ref="C41:D66" si="4">(C8/C$6)*C$39</f>
+        <f t="shared" ref="C41:D66" si="5">(C8/C$6)*C$39</f>
         <v>8.5969171441702366E-2</v>
       </c>
       <c r="D41" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.5937613479915451E-2</v>
       </c>
       <c r="E41" s="18">
-        <f t="shared" ref="E41" si="5">(E8/E$6)*E$39</f>
+        <f t="shared" ref="E41" si="6">(E8/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="18">
-        <f t="shared" ref="G41:H66" si="6">(G8/G$6)*G$39</f>
+        <f t="shared" ref="G41:H66" si="7">(G8/G$6)*G$39</f>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H41" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I41" s="18">
-        <f t="shared" ref="I41" si="7">(I8/I$6)*I$39</f>
+        <f t="shared" ref="I41" si="8">(I8/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J41" s="9">
-        <f t="shared" ref="J41:J66" si="8">G41-H41</f>
+        <f t="shared" ref="J41:J66" si="9">G41-H41</f>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L41" s="9">
@@ -3758,46 +4071,46 @@
         <v>0</v>
       </c>
       <c r="Q41" s="18">
-        <f t="shared" ref="Q41:Q66" si="9">SUM(C41:P41)</f>
+        <f t="shared" ref="Q41:Q66" si="10">SUM(C41:P41)</f>
         <v>0.27212873810004518</v>
       </c>
       <c r="R41">
-        <f t="shared" ref="R41:R66" si="10">RANK(Q41, $Q$40:$Q$66)</f>
+        <f t="shared" ref="R41:R66" si="11">RANK(Q41, $Q$40:$Q$66)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="42" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>03_Hoosier_16x6.0-10_R20_6Rim.tir</v>
       </c>
       <c r="C42" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3840351101840072E-2</v>
       </c>
       <c r="D42" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3659652863554756E-2</v>
       </c>
       <c r="E42" s="18">
-        <f t="shared" ref="E42" si="11">(E9/E$6)*E$39</f>
+        <f t="shared" ref="E42" si="12">(E9/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H42" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I42" s="18">
-        <f t="shared" ref="I42" si="12">(I9/I$6)*I$39</f>
+        <f t="shared" ref="I42" si="13">(I9/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J42" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L42" s="9">
@@ -3805,46 +4118,46 @@
         <v>0</v>
       </c>
       <c r="Q42" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.26772195714382224</v>
       </c>
       <c r="R42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="43" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>04_Hoosier_16x6.0-10_R20_7Rim.tir</v>
       </c>
       <c r="C43" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.4691923539255046E-2</v>
       </c>
       <c r="D43" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.512136694633482E-2</v>
       </c>
       <c r="E43" s="18">
-        <f t="shared" ref="E43" si="13">(E10/E$6)*E$39</f>
+        <f t="shared" ref="E43" si="14">(E10/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H43" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I43" s="18">
-        <f t="shared" ref="I43" si="14">(I10/I$6)*I$39</f>
+        <f t="shared" ref="I43" si="15">(I10/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J43" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L43" s="9">
@@ -3852,46 +4165,46 @@
         <v>0</v>
       </c>
       <c r="Q43" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.27003524366401727</v>
       </c>
       <c r="R43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="44" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
       </c>
       <c r="C44" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.0701163176186442E-2</v>
       </c>
       <c r="D44" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1506273588186748E-2</v>
       </c>
       <c r="E44" s="18">
-        <f t="shared" ref="E44" si="15">(E11/E$6)*E$39</f>
+        <f t="shared" ref="E44" si="16">(E11/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.14693343085069821</v>
       </c>
       <c r="H44" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19568120842658754</v>
       </c>
       <c r="I44" s="18">
-        <f t="shared" ref="I44" si="16">(I11/I$6)*I$39</f>
+        <f t="shared" ref="I44" si="17">(I11/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J44" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.8747777575889328E-2</v>
       </c>
       <c r="L44" s="9">
@@ -3899,46 +4212,46 @@
         <v>0</v>
       </c>
       <c r="Q44" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.57607429846576963</v>
       </c>
       <c r="R44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="45" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
       </c>
       <c r="C45" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.0506438475005155E-2</v>
       </c>
       <c r="D45" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.0638489731374214E-2</v>
       </c>
       <c r="E45" s="18">
-        <f t="shared" ref="E45" si="17">(E12/E$6)*E$39</f>
+        <f t="shared" ref="E45" si="18">(E12/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.13884333655230871</v>
       </c>
       <c r="H45" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.18426431582827674</v>
       </c>
       <c r="I45" s="18">
-        <f t="shared" ref="I45" si="18">(I12/I$6)*I$39</f>
+        <f t="shared" ref="I45" si="19">(I12/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J45" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.5420979275968026E-2</v>
       </c>
       <c r="L45" s="9">
@@ -3946,46 +4259,46 @@
         <v>0</v>
       </c>
       <c r="Q45" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.55883160131099685</v>
       </c>
       <c r="R45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="46" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>07_Goodyear_18.0x6.5-10_D0571_6Rim.tir</v>
       </c>
       <c r="C46" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.2796102078538778E-2</v>
       </c>
       <c r="D46" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.3283708989341796E-2</v>
       </c>
       <c r="E46" s="18">
-        <f t="shared" ref="E46" si="19">(E13/E$6)*E$39</f>
+        <f t="shared" ref="E46" si="20">(E13/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.15</v>
       </c>
       <c r="H46" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.2</v>
       </c>
       <c r="I46" s="18">
-        <f t="shared" ref="I46" si="20">(I13/I$6)*I$39</f>
+        <f t="shared" ref="I46" si="21">(I13/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J46" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-5.0000000000000017E-2</v>
       </c>
       <c r="L46" s="9">
@@ -3993,46 +4306,46 @@
         <v>0</v>
       </c>
       <c r="Q46" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.58607981106788065</v>
       </c>
       <c r="R46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="47" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>08_Goodyear_18.0x6.5-10_D0571_7Rim.tir</v>
       </c>
       <c r="C47" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.9480527151488951E-2</v>
       </c>
       <c r="D47" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.9274178552903108E-2</v>
       </c>
       <c r="E47" s="18">
-        <f t="shared" ref="E47" si="21">(E14/E$6)*E$39</f>
+        <f t="shared" ref="E47" si="22">(E14/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.14782263718082272</v>
       </c>
       <c r="H47" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19574602306017508</v>
       </c>
       <c r="I47" s="18">
-        <f t="shared" ref="I47" si="22">(I14/I$6)*I$39</f>
+        <f t="shared" ref="I47" si="23">(I14/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J47" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.7923385879352354E-2</v>
       </c>
       <c r="L47" s="9">
@@ -4040,46 +4353,46 @@
         <v>0</v>
       </c>
       <c r="Q47" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.57439998006603754</v>
       </c>
       <c r="R47">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="48" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>09_MRF_18x6-10_ZTD1_6Rim.tir</v>
       </c>
       <c r="C48" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.9072095902446826E-2</v>
       </c>
       <c r="D48" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8936857845982802E-2</v>
       </c>
       <c r="E48" s="18">
-        <f t="shared" ref="E48" si="23">(E15/E$6)*E$39</f>
+        <f t="shared" ref="E48" si="24">(E15/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.1166965173310599</v>
       </c>
       <c r="H48" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.15415466805458508</v>
       </c>
       <c r="I48" s="18">
-        <f t="shared" ref="I48" si="24">(I15/I$6)*I$39</f>
+        <f t="shared" ref="I48" si="25">(I15/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J48" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.745815072352518E-2</v>
       </c>
       <c r="L48" s="9">
@@ -4087,46 +4400,46 @@
         <v>0</v>
       </c>
       <c r="Q48" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.47140198841054948</v>
       </c>
       <c r="R48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="49" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10_MRF_18x6-10_ZTD1_7Rim.tir</v>
       </c>
       <c r="C49" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.5866841726526001E-2</v>
       </c>
       <c r="D49" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.5367779505210805E-2</v>
       </c>
       <c r="E49" s="18">
-        <f t="shared" ref="E49" si="25">(E16/E$6)*E$39</f>
+        <f t="shared" ref="E49" si="26">(E16/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.12182989977463995</v>
       </c>
       <c r="H49" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.16244043921238072</v>
       </c>
       <c r="I49" s="18">
-        <f t="shared" ref="I49" si="26">(I16/I$6)*I$39</f>
+        <f t="shared" ref="I49" si="27">(I16/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J49" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.0610539437740761E-2</v>
       </c>
       <c r="L49" s="9">
@@ -4134,46 +4447,46 @@
         <v>0</v>
       </c>
       <c r="Q49" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.47489442078101674</v>
       </c>
       <c r="R49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="50" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11_Hoosier_20.5x7-13_R20_7Rim.tir</v>
       </c>
       <c r="C50" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1515448327912516E-2</v>
       </c>
       <c r="D50" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1902760920824556E-2</v>
       </c>
       <c r="E50" s="18">
-        <f t="shared" ref="E50" si="27">(E17/E$6)*E$39</f>
+        <f t="shared" ref="E50" si="28">(E17/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.14436511001220323</v>
       </c>
       <c r="H50" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19099235769344683</v>
       </c>
       <c r="I50" s="18">
-        <f t="shared" ref="I50" si="28">(I17/I$6)*I$39</f>
+        <f t="shared" ref="I50" si="29">(I17/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J50" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.66272476812436E-2</v>
       </c>
       <c r="L50" s="9">
@@ -4181,46 +4494,46 @@
         <v>0</v>
       </c>
       <c r="Q50" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.57214842927314347</v>
       </c>
       <c r="R50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="51" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12_Hoosier_20.5x7-13_R20_8Rim.tir</v>
       </c>
       <c r="C51" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.7991118001788104E-2</v>
       </c>
       <c r="D51" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.8117451272981595E-2</v>
       </c>
       <c r="E51" s="18">
-        <f t="shared" ref="E51" si="29">(E18/E$6)*E$39</f>
+        <f t="shared" ref="E51" si="30">(E18/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.1427896923128783</v>
       </c>
       <c r="H51" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.18936215016976607</v>
       </c>
       <c r="I51" s="18">
-        <f t="shared" ref="I51" si="30">(I18/I$6)*I$39</f>
+        <f t="shared" ref="I51" si="31">(I18/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J51" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.6572457856887767E-2</v>
       </c>
       <c r="L51" s="9">
@@ -4228,46 +4541,46 @@
         <v>0</v>
       </c>
       <c r="Q51" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.56168795390052628</v>
       </c>
       <c r="R51">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="52" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13_Goodyear_20.0x7-13_D2704_7Rim.tir</v>
       </c>
       <c r="C52" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="D52" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
       <c r="E52" s="18">
-        <f t="shared" ref="E52" si="31">(E19/E$6)*E$39</f>
+        <f t="shared" ref="E52" si="32">(E19/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.13638040506473476</v>
       </c>
       <c r="H52" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.18038768020511103</v>
       </c>
       <c r="I52" s="18">
-        <f t="shared" ref="I52" si="32">(I19/I$6)*I$39</f>
+        <f t="shared" ref="I52" si="33">(I19/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J52" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.4007275140376279E-2</v>
       </c>
       <c r="L52" s="9">
@@ -4275,46 +4588,46 @@
         <v>0</v>
       </c>
       <c r="Q52" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.57276081012946956</v>
       </c>
       <c r="R52">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="53" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14_Goodyear_20.0x7-13_D2704_8Rim.tir</v>
       </c>
       <c r="C53" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.8167573104681263E-2</v>
       </c>
       <c r="D53" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.8142266250215165E-2</v>
       </c>
       <c r="E53" s="18">
-        <f t="shared" ref="E53" si="33">(E20/E$6)*E$39</f>
+        <f t="shared" ref="E53" si="34">(E20/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.14093524915856256</v>
       </c>
       <c r="H53" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.18592755655512896</v>
       </c>
       <c r="I53" s="18">
-        <f t="shared" ref="I53" si="34">(I20/I$6)*I$39</f>
+        <f t="shared" ref="I53" si="35">(I20/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J53" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.49923073965664E-2</v>
       </c>
       <c r="L53" s="9">
@@ -4322,46 +4635,46 @@
         <v>0</v>
       </c>
       <c r="Q53" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.55818033767202158</v>
       </c>
       <c r="R53">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="54" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15_Continental_205x470R-13_FS43329_7Rim.tir</v>
       </c>
       <c r="C54" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.892763676770519E-2</v>
       </c>
       <c r="D54" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.9998271846038114E-2</v>
       </c>
       <c r="E54" s="18">
-        <f t="shared" ref="E54" si="35">(E21/E$6)*E$39</f>
+        <f t="shared" ref="E54" si="36">(E21/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.14397095687132108</v>
       </c>
       <c r="H54" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.18998385963667339</v>
       </c>
       <c r="I54" s="18">
-        <f t="shared" ref="I54" si="36">(I21/I$6)*I$39</f>
+        <f t="shared" ref="I54" si="37">(I21/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J54" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.6012902765352304E-2</v>
       </c>
       <c r="L54" s="9">
@@ -4369,46 +4682,46 @@
         <v>0</v>
       </c>
       <c r="Q54" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.58686782235638557</v>
       </c>
       <c r="R54">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="55" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
       </c>
       <c r="C55" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.5475157106281896E-2</v>
       </c>
       <c r="D55" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.6621372449568385E-2</v>
       </c>
       <c r="E55" s="18">
-        <f t="shared" ref="E55" si="37">(E22/E$6)*E$39</f>
+        <f t="shared" ref="E55" si="38">(E22/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H55" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I55" s="18">
-        <f t="shared" ref="I55" si="38">(I22/I$6)*I$39</f>
+        <f t="shared" ref="I55" si="39">(I22/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J55" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L55" s="9">
@@ -4416,46 +4729,46 @@
         <v>0</v>
       </c>
       <c r="Q55" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.27231848273427767</v>
       </c>
       <c r="R55">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="56" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17_Hoosier_16.0x6.0-10_LCO_7Rim.tir</v>
       </c>
       <c r="C56" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.5085790915446324E-2</v>
       </c>
       <c r="D56" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.5952165358727517E-2</v>
       </c>
       <c r="E56" s="18">
-        <f t="shared" ref="E56" si="39">(E23/E$6)*E$39</f>
+        <f t="shared" ref="E56" si="40">(E23/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H56" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I56" s="18">
-        <f t="shared" ref="I56" si="40">(I23/I$6)*I$39</f>
+        <f t="shared" ref="I56" si="41">(I23/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J56" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L56" s="9">
@@ -4463,46 +4776,46 @@
         <v>0</v>
       </c>
       <c r="Q56" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.2712599094526012</v>
       </c>
       <c r="R56">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="57" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18_Hoosier_16.0x7.5-10_LCO_8Rim.tir</v>
       </c>
       <c r="C57" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.4395730566978217E-2</v>
       </c>
       <c r="D57" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.5051752110366183E-2</v>
       </c>
       <c r="E57" s="18">
-        <f t="shared" ref="E57" si="41">(E24/E$6)*E$39</f>
+        <f t="shared" ref="E57" si="42">(E24/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H57" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I57" s="18">
-        <f t="shared" ref="I57" si="42">(I24/I$6)*I$39</f>
+        <f t="shared" ref="I57" si="43">(I24/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J57" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L57" s="9">
@@ -4510,46 +4823,46 @@
         <v>0</v>
       </c>
       <c r="Q57" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.2696694358557718</v>
       </c>
       <c r="R57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="58" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
       </c>
       <c r="C58" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.4953134322792154E-2</v>
       </c>
       <c r="D58" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.5264906541803243E-2</v>
       </c>
       <c r="E58" s="18">
-        <f t="shared" ref="E58" si="43">(E25/E$6)*E$39</f>
+        <f t="shared" ref="E58" si="44">(E25/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H58" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I58" s="18">
-        <f t="shared" ref="I58" si="44">(I25/I$6)*I$39</f>
+        <f t="shared" ref="I58" si="45">(I25/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J58" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L58" s="9">
@@ -4557,46 +4870,46 @@
         <v>0</v>
       </c>
       <c r="Q58" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.27043999404302282</v>
       </c>
       <c r="R58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="59" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
       </c>
       <c r="C59" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.5503027774502365E-2</v>
       </c>
       <c r="D59" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.5955150261356311E-2</v>
       </c>
       <c r="E59" s="18">
-        <f t="shared" ref="E59" si="45">(E26/E$6)*E$39</f>
+        <f t="shared" ref="E59" si="46">(E26/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H59" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I59" s="18">
-        <f t="shared" ref="I59" si="46">(I26/I$6)*I$39</f>
+        <f t="shared" ref="I59" si="47">(I26/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J59" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L59" s="9">
@@ -4604,46 +4917,46 @@
         <v>0</v>
       </c>
       <c r="Q59" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.25168013121428606</v>
       </c>
       <c r="R59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="60" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21_Avon_7.0x16.0-11_FS_8Rim.tir</v>
       </c>
       <c r="C60" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.600961531817331E-2</v>
       </c>
       <c r="D60" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.6859328424266682E-2</v>
       </c>
       <c r="E60" s="18">
-        <f t="shared" ref="E60" si="47">(E27/E$6)*E$39</f>
+        <f t="shared" ref="E60" si="48">(E27/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.1097658921370147E-4</v>
       </c>
       <c r="H60" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.7636143842616155E-4</v>
       </c>
       <c r="I60" s="18">
-        <f t="shared" ref="I60" si="48">(I27/I$6)*I$39</f>
+        <f t="shared" ref="I60" si="49">(I27/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J60" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-6.5384849212460073E-5</v>
       </c>
       <c r="L60" s="9">
@@ -4651,46 +4964,46 @@
         <v>0</v>
       </c>
       <c r="Q60" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.25309089692086734</v>
       </c>
       <c r="R60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="61" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
       </c>
       <c r="C61" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3496431846760019E-2</v>
       </c>
       <c r="D61" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3122927066387256E-2</v>
       </c>
       <c r="E61" s="18">
-        <f t="shared" ref="E61" si="49">(E28/E$6)*E$39</f>
+        <f t="shared" ref="E61" si="50">(E28/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.14362251398065209</v>
       </c>
       <c r="H61" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19075907339485401</v>
       </c>
       <c r="I61" s="18">
-        <f t="shared" ref="I61" si="50">(I28/I$6)*I$39</f>
+        <f t="shared" ref="I61" si="51">(I28/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J61" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.7136559414201917E-2</v>
       </c>
       <c r="L61" s="9">
@@ -4698,46 +5011,46 @@
         <v>0</v>
       </c>
       <c r="Q61" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.55386438687445139</v>
       </c>
       <c r="R61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="62" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23_Avon_8.2x20.0-14_FS_9Rim.tir</v>
       </c>
       <c r="C62" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.9490291501245508E-2</v>
       </c>
       <c r="D62" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.9078111203323601E-2</v>
       </c>
       <c r="E62" s="18">
-        <f t="shared" ref="E62" si="51">(E29/E$6)*E$39</f>
+        <f t="shared" ref="E62" si="52">(E29/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.14369618433092321</v>
       </c>
       <c r="H62" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.19140458372899113</v>
       </c>
       <c r="I62" s="18">
-        <f t="shared" ref="I62" si="52">(I29/I$6)*I$39</f>
+        <f t="shared" ref="I62" si="53">(I29/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J62" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.7708399398067924E-2</v>
       </c>
       <c r="L62" s="9">
@@ -4745,46 +5058,46 @@
         <v>0</v>
       </c>
       <c r="Q62" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.54596077136641563</v>
       </c>
       <c r="R62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="63" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
       </c>
       <c r="C63" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.5795737250922493E-2</v>
       </c>
       <c r="D63" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.5631128679602116E-2</v>
       </c>
       <c r="E63" s="18">
-        <f t="shared" ref="E63" si="53">(E30/E$6)*E$39</f>
+        <f t="shared" ref="E63" si="54">(E30/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.11913295582440016</v>
       </c>
       <c r="H63" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.15652706376446146</v>
       </c>
       <c r="I63" s="18">
-        <f t="shared" ref="I63" si="54">(I30/I$6)*I$39</f>
+        <f t="shared" ref="I63" si="55">(I30/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J63" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.7394107940061302E-2</v>
       </c>
       <c r="L63" s="9">
@@ -4792,46 +5105,46 @@
         <v>0</v>
       </c>
       <c r="Q63" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.48969277757932489</v>
       </c>
       <c r="R63">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="64" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
       </c>
       <c r="C64" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.3265636100518658E-2</v>
       </c>
       <c r="D64" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.316432212859332E-2</v>
       </c>
       <c r="E64" s="18">
-        <f t="shared" ref="E64" si="55">(E31/E$6)*E$39</f>
+        <f t="shared" ref="E64" si="56">(E31/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.13137923015190839</v>
       </c>
       <c r="H64" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.17360668687005829</v>
       </c>
       <c r="I64" s="18">
-        <f t="shared" ref="I64" si="56">(I31/I$6)*I$39</f>
+        <f t="shared" ref="I64" si="57">(I31/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J64" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-4.2227456718149897E-2</v>
       </c>
       <c r="L64" s="9">
@@ -4839,46 +5152,46 @@
         <v>0</v>
       </c>
       <c r="Q64" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.50918841853292884</v>
       </c>
       <c r="R64">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="65" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
       </c>
       <c r="C65" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8951997383404975E-2</v>
       </c>
       <c r="D65" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8602030638405975E-2</v>
       </c>
       <c r="E65" s="18">
-        <f t="shared" ref="E65" si="57">(E32/E$6)*E$39</f>
+        <f t="shared" ref="E65" si="58">(E32/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.1171597320301143</v>
       </c>
       <c r="H65" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.15425287491639006</v>
       </c>
       <c r="I65" s="18">
-        <f t="shared" ref="I65" si="58">(I32/I$6)*I$39</f>
+        <f t="shared" ref="I65" si="59">(I32/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J65" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.7093142886275757E-2</v>
       </c>
       <c r="L65" s="9">
@@ -4886,46 +5199,46 @@
         <v>0</v>
       </c>
       <c r="Q65" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.47187349208203955</v>
       </c>
       <c r="R65">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="66" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27_Avon_6.2x20.0-14_FS_7Rim.tir</v>
       </c>
       <c r="C66" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.8122595570524107E-2</v>
       </c>
       <c r="D66" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.7234564689984981E-2</v>
       </c>
       <c r="E66" s="18">
-        <f t="shared" ref="E66" si="59">(E33/E$6)*E$39</f>
+        <f t="shared" ref="E66" si="60">(E33/E$6)*E$39</f>
         <v>0.1</v>
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.12060925626935157</v>
       </c>
       <c r="H66" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.15864699826663209</v>
       </c>
       <c r="I66" s="18">
-        <f t="shared" ref="I66" si="60">(I33/I$6)*I$39</f>
+        <f t="shared" ref="I66" si="61">(I33/I$6)*I$39</f>
         <v>0</v>
       </c>
       <c r="J66" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-3.8037741997280522E-2</v>
       </c>
       <c r="L66" s="9">
@@ -4933,11 +5246,11 @@
         <v>0</v>
       </c>
       <c r="Q66" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.53657567279921226</v>
       </c>
       <c r="R66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
     </row>
@@ -4949,7 +5262,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -4961,7 +5274,79 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79995117038484"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E33">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color theme="9" tint="0.79995117038484"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:F33">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color theme="9" tint="0.79995117038484"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G33">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color theme="9" tint="0.79995117038484"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:H33">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color theme="9" tint="0.79995117038484"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:I33">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color theme="9" tint="0.79995117038484"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:J33">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color theme="2"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -4973,83 +5358,96 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F33">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G33">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:H33">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J33">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E33">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7:I33">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color theme="2"/>
-        <color theme="9" tint="0.79998168889431442"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9038B9-1403-4B22-9A5D-BC5487C92A60}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="52.28515625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="e">
+        <f ca="true">xlookup(A2,Sheet2!B40:B66, Sheet2!R40:R66)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added write xlsx to make_outputs func
</commit_message>
<xml_diff>
--- a/model_outputs/tyre_ranking.xlsx
+++ b/model_outputs/tyre_ranking.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_tyre_toolbox_new\model_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D90CB75-075E-4649-A690-4B43E25B65F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5C500E-72D7-4CBD-86BE-F5E26EFD6C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" fullCalcOnLoad="true"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="152" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="69">
   <si>
     <t>'SA_at_FY_max'</t>
   </si>
@@ -229,16 +229,22 @@
   </si>
   <si>
     <t>22_Avon_8.2x20.0-13_FS_8Rim.tir</t>
+  </si>
+  <si>
+    <t>21_Avon_7.0x16.0-10_FS_8Rim.tir</t>
+  </si>
+  <si>
+    <t>23_Avon_8.2x20.0-13_FS_9Rim.tir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -375,59 +381,57 @@
       </bottom>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +450,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -597,7 +601,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -621,9 +625,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -647,7 +651,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -682,7 +686,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -700,7 +704,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -725,7 +729,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -761,56 +765,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="F15:G31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="40.875" customWidth="true"/>
-    <col min="3" max="3" width="14.5" customWidth="true"/>
-    <col min="4" max="4" width="15" customWidth="true"/>
-    <col min="5" max="5" width="22.875" customWidth="true"/>
-    <col min="6" max="6" width="17" customWidth="true"/>
-    <col min="7" max="7" width="15.375" customWidth="true"/>
-    <col min="8" max="8" width="13.125" customWidth="true"/>
-    <col min="9" max="9" width="13.375" customWidth="true"/>
-    <col min="10" max="10" width="11.625" customWidth="true"/>
-    <col min="11" max="11" width="14.625" customWidth="true"/>
-    <col min="12" max="12" width="15" customWidth="true"/>
-    <col min="13" max="13" width="14.75" bestFit="true" customWidth="true"/>
-    <col min="14" max="14" width="17" bestFit="true" customWidth="true"/>
-    <col min="15" max="15" width="23.125" customWidth="true"/>
-    <col min="16" max="22" width="12.28515625" customWidth="true"/>
-    <col min="23" max="23" width="11.28515625" customWidth="true"/>
-    <col min="24" max="24" width="12.28515625" customWidth="true"/>
-    <col min="25" max="33" width="11.5703125" customWidth="true"/>
-    <col min="34" max="34" width="10.5703125" customWidth="true"/>
-    <col min="35" max="36" width="11.5703125" customWidth="true"/>
-    <col min="37" max="37" width="10.5703125" customWidth="true"/>
-    <col min="38" max="38" width="9.5703125" customWidth="true"/>
-    <col min="39" max="55" width="11.5703125" customWidth="true"/>
-    <col min="56" max="56" width="10.5703125" customWidth="true"/>
-    <col min="57" max="77" width="11.5703125" customWidth="true"/>
-    <col min="78" max="78" width="10.5703125" customWidth="true"/>
-    <col min="79" max="90" width="11.5703125" customWidth="true"/>
-    <col min="91" max="91" width="10.5703125" customWidth="true"/>
-    <col min="92" max="98" width="11.5703125" customWidth="true"/>
-    <col min="99" max="103" width="12.28515625" customWidth="true"/>
-    <col min="104" max="104" width="11.28515625" customWidth="true"/>
-    <col min="105" max="105" width="12.28515625" customWidth="true"/>
-    <col min="106" max="106" width="10.28515625" customWidth="true"/>
-    <col min="107" max="107" width="10.5703125" customWidth="true"/>
-    <col min="108" max="110" width="2.140625" customWidth="true"/>
-    <col min="111" max="111" width="11.5703125" customWidth="true"/>
-    <col min="113" max="113" width="11.5703125" customWidth="true"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" customWidth="1"/>
+    <col min="16" max="22" width="12.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="25" max="33" width="11.5703125" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" customWidth="1"/>
+    <col min="35" max="36" width="11.5703125" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" customWidth="1"/>
+    <col min="39" max="55" width="11.5703125" customWidth="1"/>
+    <col min="56" max="56" width="10.5703125" customWidth="1"/>
+    <col min="57" max="77" width="11.5703125" customWidth="1"/>
+    <col min="78" max="78" width="10.5703125" customWidth="1"/>
+    <col min="79" max="90" width="11.5703125" customWidth="1"/>
+    <col min="91" max="91" width="10.5703125" customWidth="1"/>
+    <col min="92" max="98" width="11.5703125" customWidth="1"/>
+    <col min="99" max="103" width="12.28515625" customWidth="1"/>
+    <col min="104" max="104" width="11.28515625" customWidth="1"/>
+    <col min="105" max="105" width="12.28515625" customWidth="1"/>
+    <col min="106" max="106" width="10.28515625" customWidth="1"/>
+    <col min="107" max="107" width="10.5703125" customWidth="1"/>
+    <col min="108" max="110" width="2.140625" customWidth="1"/>
+    <col min="111" max="111" width="11.5703125" customWidth="1"/>
+    <col min="113" max="113" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -857,7 +861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -865,7 +869,7 @@
         <v>46</v>
       </c>
       <c r="C2">
-        <v>0.20319999999999999</v>
+        <v>5.4204243999999999</v>
       </c>
       <c r="D2">
         <v>-9.545454545454545</v>
@@ -904,7 +908,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -912,7 +916,7 @@
         <v>48</v>
       </c>
       <c r="C3">
-        <v>0.20319999999999999</v>
+        <v>5.5655738399999999</v>
       </c>
       <c r="D3">
         <v>-11.363636363636363</v>
@@ -951,7 +955,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -959,7 +963,7 @@
         <v>49</v>
       </c>
       <c r="C4">
-        <v>0.20319999999999999</v>
+        <v>5.0824983599999998</v>
       </c>
       <c r="D4">
         <v>-11.363636363636363</v>
@@ -998,7 +1002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1006,7 +1010,7 @@
         <v>50</v>
       </c>
       <c r="C5">
-        <v>0.20319999999999999</v>
+        <v>5.3591894799999995</v>
       </c>
       <c r="D5">
         <v>-12.878787878787877</v>
@@ -1045,7 +1049,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1053,7 +1057,7 @@
         <v>51</v>
       </c>
       <c r="C6">
-        <v>0.2286</v>
+        <v>5.5066068800000005</v>
       </c>
       <c r="D6">
         <v>-8.6363636363636367</v>
@@ -1092,7 +1096,7 @@
         <v>10.757575757575756</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1100,7 +1104,7 @@
         <v>45</v>
       </c>
       <c r="C7">
-        <v>0.2286</v>
+        <v>5.7402067599999995</v>
       </c>
       <c r="D7">
         <v>-9.545454545454545</v>
@@ -1133,7 +1137,7 @@
         <v>1199.7725693945349</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1141,7 +1145,7 @@
         <v>52</v>
       </c>
       <c r="C8">
-        <v>0.2286</v>
+        <v>5.7061873599999995</v>
       </c>
       <c r="D8">
         <v>-7.7272727272727275</v>
@@ -1180,54 +1184,54 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
-      <c r="A9" s="0">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="0">
-        <v>0.2286</v>
-      </c>
-      <c r="D9" s="0">
+      <c r="C9">
+        <v>6.0010221599999998</v>
+      </c>
+      <c r="D9">
         <v>-8.0303030303030294</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>1471.3046997420386</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>-8.0303030303030294</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>1411.2528618203514</v>
       </c>
-      <c r="H9" s="0">
+      <c r="H9">
         <v>29984.432518291324</v>
       </c>
-      <c r="I9" s="0">
-        <v>1</v>
-      </c>
-      <c r="J9" s="0">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>13.493771969144149</v>
       </c>
-      <c r="K9" s="0">
+      <c r="K9">
         <v>13.493771969144149</v>
       </c>
-      <c r="L9" s="0">
+      <c r="L9">
         <v>1332.0164029926066</v>
       </c>
-      <c r="M9" s="0">
+      <c r="M9">
         <v>6.2121212121212119</v>
       </c>
-      <c r="N9" s="0">
+      <c r="N9">
         <v>1276.6570728092877</v>
       </c>
-      <c r="O9" s="0">
+      <c r="O9">
         <v>6.2121212121212119</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1235,7 +1239,7 @@
         <v>54</v>
       </c>
       <c r="C10">
-        <v>0.2286</v>
+        <v>5.8921600799999991</v>
       </c>
       <c r="D10">
         <v>-4.3939393939393936</v>
@@ -1274,7 +1278,7 @@
         <v>4.3939393939393936</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1282,7 +1286,7 @@
         <v>55</v>
       </c>
       <c r="C11">
-        <v>0.2286</v>
+        <v>6.1461715999999997</v>
       </c>
       <c r="D11">
         <v>-4.3939393939393936</v>
@@ -1321,7 +1325,7 @@
         <v>8.9393939393939377</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1329,7 +1333,7 @@
         <v>56</v>
       </c>
       <c r="C12">
-        <v>0.26034999999999997</v>
+        <v>13.66219104</v>
       </c>
       <c r="D12">
         <v>-7.1212121212121202</v>
@@ -1368,7 +1372,7 @@
         <v>8.0303030303030294</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1376,7 +1380,7 @@
         <v>57</v>
       </c>
       <c r="C13">
-        <v>0.26034999999999997</v>
+        <v>11.902254079999999</v>
       </c>
       <c r="D13">
         <v>-5.9090909090909092</v>
@@ -1415,7 +1419,7 @@
         <v>7.7272727272727275</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1423,7 +1427,7 @@
         <v>58</v>
       </c>
       <c r="C14">
-        <v>0.254</v>
+        <v>12.163069480000001</v>
       </c>
       <c r="D14">
         <v>-9.8484848484848477</v>
@@ -1462,7 +1466,7 @@
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1470,7 +1474,7 @@
         <v>59</v>
       </c>
       <c r="C15">
-        <v>0.254</v>
+        <v>10.40086456</v>
       </c>
       <c r="D15">
         <v>-12.272727272727272</v>
@@ -1509,7 +1513,7 @@
         <v>7.1212121212121202</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1517,7 +1521,7 @@
         <v>60</v>
       </c>
       <c r="C16">
-        <v>0.20497799999999999</v>
+        <v>11.929469599999999</v>
       </c>
       <c r="D16">
         <v>-9.545454545454545</v>
@@ -1556,7 +1560,7 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1564,7 +1568,7 @@
         <v>61</v>
       </c>
       <c r="C17">
-        <v>0.20319999999999999</v>
+        <v>5.1323934799999993</v>
       </c>
       <c r="D17">
         <v>-12.272727272727272</v>
@@ -1603,7 +1607,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>62</v>
       </c>
       <c r="C18">
-        <v>0.20319999999999999</v>
+        <v>5.3047584399999996</v>
       </c>
       <c r="D18">
         <v>-9.545454545454545</v>
@@ -1650,7 +1654,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1658,7 +1662,7 @@
         <v>63</v>
       </c>
       <c r="C19">
-        <v>0.20319999999999999</v>
+        <v>5.6971155200000005</v>
       </c>
       <c r="D19">
         <v>-14.696969696969697</v>
@@ -1697,7 +1701,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1705,7 +1709,7 @@
         <v>64</v>
       </c>
       <c r="C20">
-        <v>0.20319999999999999</v>
+        <v>5.7515465599999995</v>
       </c>
       <c r="D20">
         <v>-13.181818181818182</v>
@@ -1744,7 +1748,7 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1752,7 +1756,7 @@
         <v>65</v>
       </c>
       <c r="C21">
-        <v>0.20319999999999999</v>
+        <v>5.5179466799999997</v>
       </c>
       <c r="D21">
         <v>-9.545454545454545</v>
@@ -1791,7 +1795,54 @@
         <v>47</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22">
+        <v>5.6086650799999997</v>
+      </c>
+      <c r="D22">
+        <v>-10.15151515151515</v>
+      </c>
+      <c r="E22">
+        <v>1249.8060505821679</v>
+      </c>
+      <c r="F22">
+        <v>-10.15151515151515</v>
+      </c>
+      <c r="G22">
+        <v>1202.8817765036304</v>
+      </c>
+      <c r="H22">
+        <v>20378.311960636642</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>17.482874706220215</v>
+      </c>
+      <c r="K22">
+        <v>17.482874706220215</v>
+      </c>
+      <c r="L22" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" t="s">
+        <v>47</v>
+      </c>
+      <c r="N22" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1799,7 +1850,7 @@
         <v>66</v>
       </c>
       <c r="C23">
-        <v>0.20319999999999999</v>
+        <v>11.93854144</v>
       </c>
       <c r="D23">
         <v>-14.999999999999998</v>
@@ -1838,7 +1889,54 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24">
+        <v>11.981632679999999</v>
+      </c>
+      <c r="D24">
+        <v>-13.181818181818182</v>
+      </c>
+      <c r="E24">
+        <v>1307.0378907317493</v>
+      </c>
+      <c r="F24">
+        <v>-12.878787878787877</v>
+      </c>
+      <c r="G24">
+        <v>1252.7629425828798</v>
+      </c>
+      <c r="H24">
+        <v>19024.110013201633</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>15.996700898233009</v>
+      </c>
+      <c r="K24">
+        <v>15.996700898233009</v>
+      </c>
+      <c r="L24">
+        <v>1294.8333098813791</v>
+      </c>
+      <c r="M24">
+        <v>7.7272727272727275</v>
+      </c>
+      <c r="N24">
+        <v>1242.7081938396739</v>
+      </c>
+      <c r="O24">
+        <v>7.7272727272727275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1846,7 +1944,7 @@
         <v>42</v>
       </c>
       <c r="C25">
-        <v>0.20319999999999999</v>
+        <v>13.458074640000001</v>
       </c>
       <c r="D25">
         <v>-14.999999999999998</v>
@@ -1885,7 +1983,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1893,7 +1991,7 @@
         <v>43</v>
       </c>
       <c r="C26">
-        <v>0.20319999999999999</v>
+        <v>12.02925984</v>
       </c>
       <c r="D26">
         <v>-14.999999999999998</v>
@@ -1932,7 +2030,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1940,7 +2038,7 @@
         <v>44</v>
       </c>
       <c r="C27">
-        <v>0.20319999999999999</v>
+        <v>10.763738160000001</v>
       </c>
       <c r="D27">
         <v>-14.999999999999998</v>
@@ -1981,1695 +2079,1320 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9898B6A-1213-468B-847F-2F72FED041C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9898B6A-1213-468B-847F-2F72FED041C5}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="F15:G31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="40.85546875" customWidth="true"/>
-    <col min="3" max="3" width="14.42578125" customWidth="true"/>
-    <col min="4" max="4" width="15" customWidth="true"/>
-    <col min="5" max="5" width="22.85546875" customWidth="true"/>
-    <col min="6" max="6" width="17" customWidth="true"/>
-    <col min="7" max="7" width="15.42578125" customWidth="true"/>
-    <col min="8" max="8" width="13.140625" customWidth="true"/>
-    <col min="9" max="9" width="13.42578125" customWidth="true"/>
-    <col min="10" max="10" width="11.5703125" customWidth="true"/>
-    <col min="11" max="11" width="14.5703125" customWidth="true"/>
-    <col min="12" max="12" width="15" customWidth="true"/>
-    <col min="13" max="13" width="14.7109375" bestFit="true" customWidth="true"/>
-    <col min="14" max="14" width="17" bestFit="true" customWidth="true"/>
-    <col min="15" max="15" width="23.140625" customWidth="true"/>
-    <col min="16" max="22" width="12.28515625" customWidth="true"/>
-    <col min="23" max="23" width="11.28515625" customWidth="true"/>
-    <col min="24" max="24" width="12.28515625" customWidth="true"/>
-    <col min="25" max="33" width="11.5703125" customWidth="true"/>
-    <col min="34" max="34" width="10.5703125" customWidth="true"/>
-    <col min="35" max="36" width="11.5703125" customWidth="true"/>
-    <col min="37" max="37" width="10.5703125" customWidth="true"/>
-    <col min="38" max="38" width="9.5703125" customWidth="true"/>
-    <col min="39" max="55" width="11.5703125" customWidth="true"/>
-    <col min="56" max="56" width="10.5703125" customWidth="true"/>
-    <col min="57" max="77" width="11.5703125" customWidth="true"/>
-    <col min="78" max="78" width="10.5703125" customWidth="true"/>
-    <col min="79" max="90" width="11.5703125" customWidth="true"/>
-    <col min="91" max="91" width="10.5703125" customWidth="true"/>
-    <col min="92" max="98" width="11.5703125" customWidth="true"/>
-    <col min="99" max="103" width="12.28515625" customWidth="true"/>
-    <col min="104" max="104" width="11.28515625" customWidth="true"/>
-    <col min="105" max="105" width="12.28515625" customWidth="true"/>
-    <col min="106" max="106" width="10.28515625" customWidth="true"/>
-    <col min="107" max="107" width="10.5703125" customWidth="true"/>
-    <col min="108" max="110" width="2.140625" customWidth="true"/>
-    <col min="111" max="111" width="11.5703125" customWidth="true"/>
-    <col min="113" max="113" width="11.5703125" customWidth="true"/>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" customWidth="1"/>
+    <col min="16" max="22" width="12.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.28515625" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="25" max="33" width="11.5703125" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" customWidth="1"/>
+    <col min="35" max="36" width="11.5703125" customWidth="1"/>
+    <col min="37" max="37" width="10.5703125" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" customWidth="1"/>
+    <col min="39" max="55" width="11.5703125" customWidth="1"/>
+    <col min="56" max="56" width="10.5703125" customWidth="1"/>
+    <col min="57" max="77" width="11.5703125" customWidth="1"/>
+    <col min="78" max="78" width="10.5703125" customWidth="1"/>
+    <col min="79" max="90" width="11.5703125" customWidth="1"/>
+    <col min="91" max="91" width="10.5703125" customWidth="1"/>
+    <col min="92" max="98" width="11.5703125" customWidth="1"/>
+    <col min="99" max="103" width="12.28515625" customWidth="1"/>
+    <col min="104" max="104" width="11.28515625" customWidth="1"/>
+    <col min="105" max="105" width="12.28515625" customWidth="1"/>
+    <col min="106" max="106" width="10.28515625" customWidth="1"/>
+    <col min="107" max="107" width="10.5703125" customWidth="1"/>
+    <col min="108" max="110" width="2.140625" customWidth="1"/>
+    <col min="111" max="111" width="11.5703125" customWidth="1"/>
+    <col min="113" max="113" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
-        <f>Sheet1!A1</f>
-        <v>'ID'</v>
-      </c>
-      <c r="B1" t="str">
-        <f>Sheet1!B1</f>
-        <v>'tyre'</v>
-      </c>
-      <c r="C1" t="str">
-        <f>Sheet1!C1</f>
-        <v>'SA_at_FY_max'</v>
-      </c>
-      <c r="D1" t="str">
-        <f>Sheet1!D1</f>
-        <v>'FY_design_max'</v>
-      </c>
-      <c r="E1" t="str">
-        <f>Sheet1!E1</f>
-        <v>'SA_at_FY_max_with_LLT'</v>
-      </c>
-      <c r="F1" t="str">
-        <f>Sheet1!F1</f>
-        <v>'FY_max_with_LLT'</v>
-      </c>
-      <c r="G1" t="str">
-        <f>Sheet1!G1</f>
-        <v>'CS_design_max'</v>
-      </c>
-      <c r="H1" t="str">
-        <f>Sheet1!H1</f>
-        <v>'CS_LLT_max'</v>
-      </c>
-      <c r="I1" t="str">
-        <f>Sheet1!I1</f>
-        <v>'load_sensitive'</v>
-      </c>
-      <c r="J1" t="str">
-        <f>Sheet1!J1</f>
-        <v>'MZ_max'</v>
-      </c>
-      <c r="K1" t="str">
-        <f>Sheet1!K1</f>
-        <v>'SA_at_max_MZ'</v>
-      </c>
-      <c r="L1" t="str">
-        <f>Sheet1!L1</f>
-        <v>'FX_design_max'</v>
-      </c>
-      <c r="M1" t="str">
-        <f>Sheet1!M1</f>
-        <v>'SR_at_FX_max'</v>
-      </c>
-      <c r="N1" t="str">
-        <f>Sheet1!N1</f>
-        <v>'FX_max_with_LLT'</v>
-      </c>
-      <c r="O1" t="str">
-        <f>Sheet1!O1</f>
-        <v>'SR_at_FX_max_with_LLT'</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>Sheet1!A2</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
       </c>
       <c r="C2">
-        <f>Sheet1!C2</f>
-        <v>0.20319999999999999</v>
+        <v>5.4204243999999999</v>
       </c>
       <c r="D2">
-        <f>Sheet1!D2</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="E2">
-        <f>Sheet1!E2</f>
         <v>1418.1229466068155</v>
       </c>
       <c r="F2">
-        <f>Sheet1!F2</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="G2">
-        <f>Sheet1!G2</f>
         <v>1361.0997873181398</v>
       </c>
       <c r="H2">
-        <f>Sheet1!H2</f>
         <v>21130.319713418798</v>
       </c>
       <c r="I2">
-        <f>Sheet1!I2</f>
         <v>1</v>
       </c>
       <c r="J2">
-        <f>Sheet1!J2</f>
         <v>23.257005658544909</v>
       </c>
       <c r="K2">
-        <f>Sheet1!K2</f>
         <v>23.257005658544909</v>
       </c>
-      <c r="L2" t="str">
-        <f>Sheet1!L2</f>
-        <v>ND</v>
-      </c>
-      <c r="M2" t="str">
-        <f>Sheet1!M2</f>
-        <v>ND</v>
-      </c>
-      <c r="N2" t="str">
-        <f>Sheet1!N2</f>
-        <v>ND</v>
-      </c>
-      <c r="O2" t="str">
-        <f>Sheet1!O2</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>Sheet1!A3</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
       </c>
       <c r="C3">
-        <f>Sheet1!C3</f>
-        <v>0.20319999999999999</v>
+        <v>5.5655738399999999</v>
       </c>
       <c r="D3">
-        <f>Sheet1!D3</f>
         <v>-11.363636363636363</v>
       </c>
       <c r="E3">
-        <f>Sheet1!E3</f>
         <v>1413.5684042290648</v>
       </c>
       <c r="F3">
-        <f>Sheet1!F3</f>
         <v>-11.666666666666664</v>
       </c>
       <c r="G3">
-        <f>Sheet1!G3</f>
         <v>1356.5084942202984</v>
       </c>
       <c r="H3">
-        <f>Sheet1!H3</f>
         <v>22460.395534030638</v>
       </c>
       <c r="I3">
-        <f>Sheet1!I3</f>
         <v>1</v>
       </c>
       <c r="J3">
-        <f>Sheet1!J3</f>
         <v>18.410277578573179</v>
       </c>
       <c r="K3">
-        <f>Sheet1!K3</f>
         <v>18.410277578573179</v>
       </c>
-      <c r="L3" t="str">
-        <f>Sheet1!L3</f>
-        <v>ND</v>
-      </c>
-      <c r="M3" t="str">
-        <f>Sheet1!M3</f>
-        <v>ND</v>
-      </c>
-      <c r="N3" t="str">
-        <f>Sheet1!N3</f>
-        <v>ND</v>
-      </c>
-      <c r="O3" t="str">
-        <f>Sheet1!O3</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>Sheet1!A4</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
       <c r="C4">
-        <f>Sheet1!C4</f>
-        <v>0.20319999999999999</v>
+        <v>5.0824983599999998</v>
       </c>
       <c r="D4">
-        <f>Sheet1!D4</f>
         <v>-11.363636363636363</v>
       </c>
       <c r="E4">
-        <f>Sheet1!E4</f>
         <v>1378.5647730407597</v>
       </c>
       <c r="F4">
-        <f>Sheet1!F4</f>
         <v>-11.363636363636363</v>
       </c>
       <c r="G4">
-        <f>Sheet1!G4</f>
         <v>1322.3308133748815</v>
       </c>
       <c r="H4">
-        <f>Sheet1!H4</f>
         <v>19143.469473247831</v>
       </c>
       <c r="I4">
-        <f>Sheet1!I4</f>
         <v>1</v>
       </c>
       <c r="J4">
-        <f>Sheet1!J4</f>
         <v>14.317499793697406</v>
       </c>
       <c r="K4">
-        <f>Sheet1!K4</f>
         <v>14.317499793697406</v>
       </c>
-      <c r="L4" t="str">
-        <f>Sheet1!L4</f>
-        <v>ND</v>
-      </c>
-      <c r="M4" t="str">
-        <f>Sheet1!M4</f>
-        <v>ND</v>
-      </c>
-      <c r="N4" t="str">
-        <f>Sheet1!N4</f>
-        <v>ND</v>
-      </c>
-      <c r="O4" t="str">
-        <f>Sheet1!O4</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>Sheet1!A5</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
       </c>
       <c r="C5">
-        <f>Sheet1!C5</f>
-        <v>0.20319999999999999</v>
+        <v>5.3591894799999995</v>
       </c>
       <c r="D5">
-        <f>Sheet1!D5</f>
         <v>-12.878787878787877</v>
       </c>
       <c r="E5">
-        <f>Sheet1!E5</f>
         <v>1392.5669539534656</v>
       </c>
       <c r="F5">
-        <f>Sheet1!F5</f>
         <v>-13.181818181818182</v>
       </c>
       <c r="G5">
-        <f>Sheet1!G5</f>
         <v>1338.2031224203297</v>
       </c>
       <c r="H5">
-        <f>Sheet1!H5</f>
         <v>19199.827902147637</v>
       </c>
       <c r="I5">
-        <f>Sheet1!I5</f>
         <v>1</v>
       </c>
       <c r="J5">
-        <f>Sheet1!J5</f>
         <v>15.387366226633146</v>
       </c>
       <c r="K5">
-        <f>Sheet1!K5</f>
         <v>15.387366226633146</v>
       </c>
-      <c r="L5" t="str">
-        <f>Sheet1!L5</f>
-        <v>ND</v>
-      </c>
-      <c r="M5" t="str">
-        <f>Sheet1!M5</f>
-        <v>ND</v>
-      </c>
-      <c r="N5" t="str">
-        <f>Sheet1!N5</f>
-        <v>ND</v>
-      </c>
-      <c r="O5" t="str">
-        <f>Sheet1!O5</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>Sheet1!A6</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
       </c>
       <c r="C6">
-        <f>Sheet1!C6</f>
-        <v>0.2286</v>
+        <v>5.5066068800000005</v>
       </c>
       <c r="D6">
-        <f>Sheet1!D6</f>
         <v>-8.6363636363636367</v>
       </c>
       <c r="E6">
-        <f>Sheet1!E6</f>
         <v>1491.375295848065</v>
       </c>
       <c r="F6">
-        <f>Sheet1!F6</f>
         <v>-8.6363636363636367</v>
       </c>
       <c r="G6">
-        <f>Sheet1!G6</f>
         <v>1434.436407162452</v>
       </c>
       <c r="H6">
-        <f>Sheet1!H6</f>
         <v>24174.206639737571</v>
       </c>
       <c r="I6">
-        <f>Sheet1!I6</f>
         <v>1</v>
       </c>
       <c r="J6">
-        <f>Sheet1!J6</f>
         <v>29.40616397091755</v>
       </c>
       <c r="K6">
-        <f>Sheet1!K6</f>
         <v>29.40616397091755</v>
       </c>
       <c r="L6">
-        <f>Sheet1!L6</f>
         <v>1324.0038452412396</v>
       </c>
       <c r="M6">
-        <f>Sheet1!M6</f>
         <v>10.454545454545455</v>
       </c>
       <c r="N6">
-        <f>Sheet1!N6</f>
         <v>1270.7848708819997</v>
       </c>
       <c r="O6">
-        <f>Sheet1!O6</f>
         <v>10.757575757575756</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>Sheet1!A7</f>
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
       </c>
       <c r="C7">
-        <f>Sheet1!C7</f>
-        <v>0.2286</v>
+        <v>5.7402067599999995</v>
       </c>
       <c r="D7">
-        <f>Sheet1!D7</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="E7">
-        <f>Sheet1!E7</f>
         <v>1488.1734889619829</v>
       </c>
       <c r="F7">
-        <f>Sheet1!F7</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="G7">
-        <f>Sheet1!G7</f>
         <v>1428.7543587969342</v>
       </c>
       <c r="H7">
-        <f>Sheet1!H7</f>
         <v>23057.299498565211</v>
       </c>
       <c r="I7">
-        <f>Sheet1!I7</f>
         <v>1</v>
       </c>
       <c r="J7">
-        <f>Sheet1!J7</f>
         <v>23.555160700712687</v>
       </c>
       <c r="K7">
-        <f>Sheet1!K7</f>
         <v>23.555160700712687</v>
       </c>
       <c r="L7">
-        <f>Sheet1!L7</f>
         <v>1251.1047378194853</v>
       </c>
-      <c r="M7">
-        <f>Sheet1!M7</f>
-        <v>0</v>
-      </c>
       <c r="N7">
-        <f>Sheet1!N7</f>
         <v>1199.7725693945349</v>
       </c>
-      <c r="O7">
-        <f>Sheet1!O7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>Sheet1!A8</f>
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
       </c>
       <c r="C8">
-        <f>Sheet1!C8</f>
-        <v>0.2286</v>
+        <v>5.7061873599999995</v>
       </c>
       <c r="D8">
-        <f>Sheet1!D8</f>
         <v>-7.7272727272727275</v>
       </c>
       <c r="E8">
-        <f>Sheet1!E8</f>
         <v>1525.8218234985466</v>
       </c>
       <c r="F8">
-        <f>Sheet1!F8</f>
         <v>-7.7272727272727275</v>
       </c>
       <c r="G8">
-        <f>Sheet1!G8</f>
         <v>1466.3146871310005</v>
       </c>
       <c r="H8">
-        <f>Sheet1!H8</f>
         <v>31087.629309098418</v>
       </c>
       <c r="I8">
-        <f>Sheet1!I8</f>
         <v>1</v>
       </c>
       <c r="J8">
-        <f>Sheet1!J8</f>
         <v>25.969275063951901</v>
       </c>
       <c r="K8">
-        <f>Sheet1!K8</f>
         <v>25.969275063951901</v>
       </c>
       <c r="L8">
-        <f>Sheet1!L8</f>
         <v>1351.6364222651798</v>
       </c>
       <c r="M8">
-        <f>Sheet1!M8</f>
         <v>5.9090909090909092</v>
       </c>
       <c r="N8">
-        <f>Sheet1!N8</f>
         <v>1297.7181145944969</v>
       </c>
       <c r="O8">
-        <f>Sheet1!O8</f>
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>Sheet1!A9</f>
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
       <c r="C9">
-        <f>Sheet1!C9</f>
-        <v>0.2286</v>
+        <v>6.0010221599999998</v>
       </c>
       <c r="D9">
-        <f>Sheet1!D9</f>
         <v>-8.0303030303030294</v>
       </c>
       <c r="E9">
-        <f>Sheet1!E9</f>
         <v>1471.3046997420386</v>
       </c>
       <c r="F9">
-        <f>Sheet1!F9</f>
         <v>-8.0303030303030294</v>
       </c>
       <c r="G9">
-        <f>Sheet1!G9</f>
         <v>1411.2528618203514</v>
       </c>
       <c r="H9">
-        <f>Sheet1!H9</f>
         <v>29984.432518291324</v>
       </c>
       <c r="I9">
-        <f>Sheet1!I9</f>
         <v>1</v>
       </c>
       <c r="J9">
-        <f>Sheet1!J9</f>
         <v>13.493771969144149</v>
       </c>
       <c r="K9">
-        <f>Sheet1!K9</f>
         <v>13.493771969144149</v>
       </c>
       <c r="L9">
-        <f>Sheet1!L9</f>
         <v>1332.0164029926066</v>
       </c>
       <c r="M9">
-        <f>Sheet1!M9</f>
         <v>6.2121212121212119</v>
       </c>
       <c r="N9">
-        <f>Sheet1!N9</f>
         <v>1276.6570728092877</v>
       </c>
       <c r="O9">
-        <f>Sheet1!O9</f>
         <v>6.2121212121212119</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>Sheet1!A10</f>
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>54</v>
       </c>
       <c r="C10">
-        <f>Sheet1!C10</f>
-        <v>0.2286</v>
+        <v>5.8921600799999991</v>
       </c>
       <c r="D10">
-        <f>Sheet1!D10</f>
         <v>-4.3939393939393936</v>
       </c>
       <c r="E10">
-        <f>Sheet1!E10</f>
         <v>1135.7342491987292</v>
       </c>
       <c r="F10">
-        <f>Sheet1!F10</f>
         <v>-4.3939393939393936</v>
       </c>
       <c r="G10">
-        <f>Sheet1!G10</f>
         <v>1089.4387408425803</v>
       </c>
       <c r="H10">
-        <f>Sheet1!H10</f>
         <v>34644.059496909038</v>
       </c>
       <c r="I10">
-        <f>Sheet1!I10</f>
         <v>1</v>
       </c>
       <c r="J10">
-        <f>Sheet1!J10</f>
         <v>13.055626098617871</v>
       </c>
       <c r="K10">
-        <f>Sheet1!K10</f>
         <v>13.055626098617871</v>
       </c>
       <c r="L10">
-        <f>Sheet1!L10</f>
         <v>1051.5417545077357</v>
       </c>
       <c r="M10">
-        <f>Sheet1!M10</f>
         <v>4.3939393939393936</v>
       </c>
       <c r="N10">
-        <f>Sheet1!N10</f>
         <v>1007.2417282539946</v>
       </c>
       <c r="O10">
-        <f>Sheet1!O10</f>
         <v>4.3939393939393936</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>Sheet1!A11</f>
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>55</v>
       </c>
       <c r="C11">
-        <f>Sheet1!C11</f>
-        <v>0.2286</v>
+        <v>6.1461715999999997</v>
       </c>
       <c r="D11">
-        <f>Sheet1!D11</f>
         <v>-4.3939393939393936</v>
       </c>
       <c r="E11">
-        <f>Sheet1!E11</f>
         <v>1083.0311004464186</v>
       </c>
       <c r="F11">
-        <f>Sheet1!F11</f>
         <v>-4.3939393939393936</v>
       </c>
       <c r="G11">
-        <f>Sheet1!G11</f>
         <v>1037.3963503362741</v>
       </c>
       <c r="H11">
-        <f>Sheet1!H11</f>
         <v>40807.883351918004</v>
       </c>
       <c r="I11">
-        <f>Sheet1!I11</f>
         <v>1</v>
       </c>
       <c r="J11">
-        <f>Sheet1!J11</f>
         <v>12.011174605197123</v>
       </c>
       <c r="K11">
-        <f>Sheet1!K11</f>
         <v>12.011174605197123</v>
       </c>
       <c r="L11">
-        <f>Sheet1!L11</f>
         <v>1097.798199042132</v>
       </c>
       <c r="M11">
-        <f>Sheet1!M11</f>
         <v>8.6363636363636367</v>
       </c>
       <c r="N11">
-        <f>Sheet1!N11</f>
         <v>1053.9942864708885</v>
       </c>
       <c r="O11">
-        <f>Sheet1!O11</f>
         <v>8.9393939393939377</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>Sheet1!A12</f>
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
       </c>
       <c r="C12">
-        <f>Sheet1!C12</f>
-        <v>0.26034999999999997</v>
+        <v>13.66219104</v>
       </c>
       <c r="D12">
-        <f>Sheet1!D12</f>
         <v>-7.1212121212121202</v>
       </c>
       <c r="E12">
-        <f>Sheet1!E12</f>
         <v>1504.7643717599271</v>
       </c>
       <c r="F12">
-        <f>Sheet1!F12</f>
         <v>-7.1212121212121202</v>
       </c>
       <c r="G12">
-        <f>Sheet1!G12</f>
         <v>1445.588586319112</v>
       </c>
       <c r="H12">
-        <f>Sheet1!H12</f>
         <v>28787.366111526724</v>
       </c>
       <c r="I12">
-        <f>Sheet1!I12</f>
         <v>1</v>
       </c>
       <c r="J12">
-        <f>Sheet1!J12</f>
         <v>2.9056529242126601</v>
       </c>
       <c r="K12">
-        <f>Sheet1!K12</f>
         <v>2.9056529242126601</v>
       </c>
       <c r="L12">
-        <f>Sheet1!L12</f>
         <v>1300.8609386454232</v>
       </c>
       <c r="M12">
-        <f>Sheet1!M12</f>
         <v>8.0303030303030294</v>
       </c>
       <c r="N12">
-        <f>Sheet1!N12</f>
         <v>1246.5415380785441</v>
       </c>
       <c r="O12">
-        <f>Sheet1!O12</f>
         <v>8.0303030303030294</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>Sheet1!A13</f>
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>57</v>
       </c>
       <c r="C13">
-        <f>Sheet1!C13</f>
-        <v>0.26034999999999997</v>
+        <v>11.902254079999999</v>
       </c>
       <c r="D13">
-        <f>Sheet1!D13</f>
         <v>-5.9090909090909092</v>
       </c>
       <c r="E13">
-        <f>Sheet1!E13</f>
         <v>1446.814738053685</v>
       </c>
       <c r="F13">
-        <f>Sheet1!F13</f>
         <v>-5.6060606060606055</v>
       </c>
       <c r="G13">
-        <f>Sheet1!G13</f>
         <v>1388.9937103022055</v>
       </c>
       <c r="H13">
-        <f>Sheet1!H13</f>
         <v>36968.755564889514</v>
       </c>
       <c r="I13">
-        <f>Sheet1!I13</f>
         <v>1</v>
       </c>
       <c r="J13">
-        <f>Sheet1!J13</f>
         <v>8.621782382758834</v>
       </c>
       <c r="K13">
-        <f>Sheet1!K13</f>
         <v>8.621782382758834</v>
       </c>
       <c r="L13">
-        <f>Sheet1!L13</f>
         <v>1286.6649923608313</v>
       </c>
       <c r="M13">
-        <f>Sheet1!M13</f>
         <v>7.7272727272727275</v>
       </c>
       <c r="N13">
-        <f>Sheet1!N13</f>
         <v>1233.6827348691093</v>
       </c>
       <c r="O13">
-        <f>Sheet1!O13</f>
         <v>7.7272727272727275</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>Sheet1!A14</f>
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>58</v>
       </c>
       <c r="C14">
-        <f>Sheet1!C14</f>
-        <v>0.254</v>
+        <v>12.163069480000001</v>
       </c>
       <c r="D14">
-        <f>Sheet1!D14</f>
         <v>-9.8484848484848477</v>
       </c>
       <c r="E14">
-        <f>Sheet1!E14</f>
         <v>1644.2736163714658</v>
       </c>
       <c r="F14">
-        <f>Sheet1!F14</f>
         <v>-9.8484848484848477</v>
       </c>
       <c r="G14">
-        <f>Sheet1!G14</f>
         <v>1578.0814183326409</v>
       </c>
       <c r="H14">
-        <f>Sheet1!H14</f>
         <v>29240.85832208081</v>
       </c>
       <c r="I14">
-        <f>Sheet1!I14</f>
         <v>1</v>
       </c>
       <c r="J14">
-        <f>Sheet1!J14</f>
         <v>22.111672740793562</v>
       </c>
       <c r="K14">
-        <f>Sheet1!K14</f>
         <v>22.111672740793562</v>
       </c>
       <c r="L14">
-        <f>Sheet1!L14</f>
         <v>1228.9114851251607</v>
       </c>
       <c r="M14">
-        <f>Sheet1!M14</f>
         <v>8.3333333333333321</v>
       </c>
       <c r="N14">
-        <f>Sheet1!N14</f>
         <v>1177.5096590958383</v>
       </c>
       <c r="O14">
-        <f>Sheet1!O14</f>
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>Sheet1!A15</f>
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>59</v>
       </c>
       <c r="C15">
-        <f>Sheet1!C15</f>
-        <v>0.254</v>
+        <v>10.40086456</v>
       </c>
       <c r="D15">
-        <f>Sheet1!D15</f>
         <v>-12.272727272727272</v>
       </c>
       <c r="E15">
-        <f>Sheet1!E15</f>
         <v>1449.7161427552983</v>
       </c>
       <c r="F15">
-        <f>Sheet1!F15</f>
         <v>-12.272727272727272</v>
       </c>
       <c r="G15">
-        <f>Sheet1!G15</f>
         <v>1391.2397600678448</v>
       </c>
       <c r="H15">
-        <f>Sheet1!H15</f>
         <v>27410.226980274612</v>
       </c>
       <c r="I15">
-        <f>Sheet1!I15</f>
         <v>1</v>
       </c>
       <c r="J15">
-        <f>Sheet1!J15</f>
         <v>13.370072921729852</v>
       </c>
       <c r="K15">
-        <f>Sheet1!K15</f>
         <v>13.370072921729852</v>
       </c>
       <c r="L15">
-        <f>Sheet1!L15</f>
         <v>1269.9547729582082</v>
       </c>
       <c r="M15">
-        <f>Sheet1!M15</f>
         <v>7.1212121212121202</v>
       </c>
       <c r="N15">
-        <f>Sheet1!N15</f>
         <v>1215.9956664122051</v>
       </c>
       <c r="O15">
-        <f>Sheet1!O15</f>
         <v>7.1212121212121202</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>Sheet1!A16</f>
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
       </c>
       <c r="C16">
-        <f>Sheet1!C16</f>
-        <v>0.20497799999999999</v>
+        <v>11.929469599999999</v>
       </c>
       <c r="D16">
-        <f>Sheet1!D16</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="E16">
-        <f>Sheet1!E16</f>
         <v>1626.6410306711739</v>
       </c>
       <c r="F16">
-        <f>Sheet1!F16</f>
         <v>-9.8484848484848477</v>
       </c>
       <c r="G16">
-        <f>Sheet1!G16</f>
         <v>1565.662677459768</v>
       </c>
       <c r="H16">
-        <f>Sheet1!H16</f>
         <v>30766.058316327431</v>
       </c>
       <c r="I16">
-        <f>Sheet1!I16</f>
         <v>1</v>
       </c>
       <c r="J16">
-        <f>Sheet1!J16</f>
         <v>13.736907144326651</v>
       </c>
       <c r="K16">
-        <f>Sheet1!K16</f>
         <v>13.736907144326651</v>
       </c>
       <c r="L16">
-        <f>Sheet1!L16</f>
         <v>1297.3092603709797</v>
       </c>
       <c r="M16">
-        <f>Sheet1!M16</f>
         <v>5.9090909090909092</v>
       </c>
       <c r="N16">
-        <f>Sheet1!N16</f>
         <v>1242.2488145572831</v>
       </c>
       <c r="O16">
-        <f>Sheet1!O16</f>
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>Sheet1!A17</f>
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
       </c>
       <c r="C17">
-        <f>Sheet1!C17</f>
-        <v>0.20319999999999999</v>
+        <v>5.1323934799999993</v>
       </c>
       <c r="D17">
-        <f>Sheet1!D17</f>
         <v>-12.272727272727272</v>
       </c>
       <c r="E17">
-        <f>Sheet1!E17</f>
         <v>1405.4454568506533</v>
       </c>
       <c r="F17">
-        <f>Sheet1!F17</f>
         <v>-12.272727272727272</v>
       </c>
       <c r="G17">
-        <f>Sheet1!G17</f>
         <v>1353.4044916495345</v>
       </c>
       <c r="H17">
-        <f>Sheet1!H17</f>
         <v>19958.48151666945</v>
       </c>
       <c r="I17">
-        <f>Sheet1!I17</f>
         <v>1</v>
       </c>
       <c r="J17">
-        <f>Sheet1!J17</f>
         <v>22.83479006064082</v>
       </c>
       <c r="K17">
-        <f>Sheet1!K17</f>
         <v>22.83479006064082</v>
       </c>
-      <c r="L17" t="str">
-        <f>Sheet1!L17</f>
-        <v>ND</v>
-      </c>
-      <c r="M17" t="str">
-        <f>Sheet1!M17</f>
-        <v>ND</v>
-      </c>
-      <c r="N17" t="str">
-        <f>Sheet1!N17</f>
-        <v>ND</v>
-      </c>
-      <c r="O17" t="str">
-        <f>Sheet1!O17</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>Sheet1!A18</f>
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>62</v>
       </c>
       <c r="C18">
-        <f>Sheet1!C18</f>
-        <v>0.20319999999999999</v>
+        <v>5.3047584399999996</v>
       </c>
       <c r="D18">
-        <f>Sheet1!D18</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="E18">
-        <f>Sheet1!E18</f>
         <v>1399.0432113036734</v>
       </c>
       <c r="F18">
-        <f>Sheet1!F18</f>
         <v>-9.2424242424242422</v>
       </c>
       <c r="G18">
-        <f>Sheet1!G18</f>
         <v>1346.1946241648366</v>
       </c>
       <c r="H18">
-        <f>Sheet1!H18</f>
         <v>21253.399390250874</v>
       </c>
       <c r="I18">
-        <f>Sheet1!I18</f>
         <v>1</v>
       </c>
       <c r="J18">
-        <f>Sheet1!J18</f>
         <v>23.060648079149942</v>
       </c>
       <c r="K18">
-        <f>Sheet1!K18</f>
         <v>23.060648079149942</v>
       </c>
-      <c r="L18" t="str">
-        <f>Sheet1!L18</f>
-        <v>ND</v>
-      </c>
-      <c r="M18" t="str">
-        <f>Sheet1!M18</f>
-        <v>ND</v>
-      </c>
-      <c r="N18" t="str">
-        <f>Sheet1!N18</f>
-        <v>ND</v>
-      </c>
-      <c r="O18" t="str">
-        <f>Sheet1!O18</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>Sheet1!A19</f>
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>63</v>
       </c>
       <c r="C19">
-        <f>Sheet1!C19</f>
-        <v>0.20319999999999999</v>
+        <v>5.6971155200000005</v>
       </c>
       <c r="D19">
-        <f>Sheet1!D19</f>
         <v>-14.696969696969697</v>
       </c>
       <c r="E19">
-        <f>Sheet1!E19</f>
         <v>1387.6967310567711</v>
       </c>
       <c r="F19">
-        <f>Sheet1!F19</f>
         <v>-14.696969696969697</v>
       </c>
       <c r="G19">
-        <f>Sheet1!G19</f>
         <v>1334.4172130966144</v>
       </c>
       <c r="H19">
-        <f>Sheet1!H19</f>
         <v>20065.804846484891</v>
       </c>
       <c r="I19">
-        <f>Sheet1!I19</f>
         <v>1</v>
       </c>
       <c r="J19">
-        <f>Sheet1!J19</f>
         <v>21.612145087895232</v>
       </c>
       <c r="K19">
-        <f>Sheet1!K19</f>
         <v>21.612145087895232</v>
       </c>
-      <c r="L19" t="str">
-        <f>Sheet1!L19</f>
-        <v>ND</v>
-      </c>
-      <c r="M19" t="str">
-        <f>Sheet1!M19</f>
-        <v>ND</v>
-      </c>
-      <c r="N19" t="str">
-        <f>Sheet1!N19</f>
-        <v>ND</v>
-      </c>
-      <c r="O19" t="str">
-        <f>Sheet1!O19</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>47</v>
+      </c>
+      <c r="M19" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>Sheet1!A20</f>
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
       </c>
       <c r="C20">
-        <f>Sheet1!C20</f>
-        <v>0.20319999999999999</v>
+        <v>5.7515465599999995</v>
       </c>
       <c r="D20">
-        <f>Sheet1!D20</f>
         <v>-13.181818181818182</v>
       </c>
       <c r="E20">
-        <f>Sheet1!E20</f>
         <v>1396.8619739502833</v>
       </c>
       <c r="F20">
-        <f>Sheet1!F20</f>
         <v>-12.878787878787877</v>
       </c>
       <c r="G20">
-        <f>Sheet1!G20</f>
         <v>1341.839498871735</v>
       </c>
       <c r="H20">
-        <f>Sheet1!H20</f>
         <v>20428.69287290483</v>
       </c>
       <c r="I20">
-        <f>Sheet1!I20</f>
         <v>1</v>
       </c>
       <c r="J20">
-        <f>Sheet1!J20</f>
         <v>22.713968065012555</v>
       </c>
       <c r="K20">
-        <f>Sheet1!K20</f>
         <v>22.713968065012555</v>
       </c>
-      <c r="L20" t="str">
-        <f>Sheet1!L20</f>
-        <v>ND</v>
-      </c>
-      <c r="M20" t="str">
-        <f>Sheet1!M20</f>
-        <v>ND</v>
-      </c>
-      <c r="N20" t="str">
-        <f>Sheet1!N20</f>
-        <v>ND</v>
-      </c>
-      <c r="O20" t="str">
-        <f>Sheet1!O20</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>47</v>
+      </c>
+      <c r="M20" t="s">
+        <v>47</v>
+      </c>
+      <c r="N20" t="s">
+        <v>47</v>
+      </c>
+      <c r="O20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>Sheet1!A21</f>
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>65</v>
       </c>
       <c r="C21">
-        <f>Sheet1!C21</f>
-        <v>0.20319999999999999</v>
+        <v>5.5179466799999997</v>
       </c>
       <c r="D21">
-        <f>Sheet1!D21</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="E21">
-        <f>Sheet1!E21</f>
         <v>1241.4763652577622</v>
       </c>
       <c r="F21">
-        <f>Sheet1!F21</f>
         <v>-9.545454545454545</v>
       </c>
       <c r="G21">
-        <f>Sheet1!G21</f>
         <v>1193.2814934266471</v>
       </c>
       <c r="H21">
-        <f>Sheet1!H21</f>
         <v>18859.597365099344</v>
       </c>
       <c r="I21">
-        <f>Sheet1!I21</f>
         <v>1</v>
       </c>
       <c r="J21">
-        <f>Sheet1!J21</f>
         <v>13.53973768766312</v>
       </c>
       <c r="K21">
-        <f>Sheet1!K21</f>
         <v>13.53973768766312</v>
       </c>
-      <c r="L21" t="str">
-        <f>Sheet1!L21</f>
-        <v>ND</v>
-      </c>
-      <c r="M21" t="str">
-        <f>Sheet1!M21</f>
-        <v>ND</v>
-      </c>
-      <c r="N21" t="str">
-        <f>Sheet1!N21</f>
-        <v>ND</v>
-      </c>
-      <c r="O21" t="str">
-        <f>Sheet1!O21</f>
-        <v>ND</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" t="s">
+        <v>47</v>
+      </c>
+      <c r="O21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>Sheet1!A22</f>
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
       </c>
       <c r="C22">
-        <f>Sheet1!C22</f>
-        <v>0</v>
+        <v>5.6086650799999997</v>
       </c>
       <c r="D22">
-        <f>Sheet1!D22</f>
-        <v>0</v>
+        <v>-10.15151515151515</v>
       </c>
       <c r="E22">
-        <f>Sheet1!E22</f>
-        <v>0</v>
+        <v>1249.8060505821679</v>
       </c>
       <c r="F22">
-        <f>Sheet1!F22</f>
-        <v>0</v>
+        <v>-10.15151515151515</v>
       </c>
       <c r="G22">
-        <f>Sheet1!G22</f>
-        <v>0</v>
+        <v>1202.8817765036304</v>
       </c>
       <c r="H22">
-        <f>Sheet1!H22</f>
-        <v>0</v>
+        <v>20378.311960636642</v>
       </c>
       <c r="I22">
-        <f>Sheet1!I22</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
-        <f>Sheet1!J22</f>
-        <v>0</v>
+        <v>17.482874706220215</v>
       </c>
       <c r="K22">
-        <f>Sheet1!K22</f>
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <f>Sheet1!L22</f>
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <f>Sheet1!M22</f>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <f>Sheet1!N22</f>
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <f>Sheet1!O22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
+        <v>17.482874706220215</v>
+      </c>
+      <c r="L22" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" t="s">
+        <v>47</v>
+      </c>
+      <c r="N22" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>Sheet1!A23</f>
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
       <c r="C23">
-        <f>Sheet1!C23</f>
-        <v>0.20319999999999999</v>
+        <v>11.93854144</v>
       </c>
       <c r="D23">
-        <f>Sheet1!D23</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="E23">
-        <f>Sheet1!E23</f>
         <v>1372.9097994678571</v>
       </c>
       <c r="F23">
-        <f>Sheet1!F23</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="G23">
-        <f>Sheet1!G23</f>
         <v>1316.155000642593</v>
       </c>
       <c r="H23">
-        <f>Sheet1!H23</f>
         <v>18597.177761836752</v>
       </c>
       <c r="I23">
-        <f>Sheet1!I23</f>
         <v>1</v>
       </c>
       <c r="J23">
-        <f>Sheet1!J23</f>
         <v>17.771256090695569</v>
       </c>
       <c r="K23">
-        <f>Sheet1!K23</f>
         <v>17.771256090695569</v>
       </c>
       <c r="L23">
-        <f>Sheet1!L23</f>
         <v>1294.1694730235959</v>
       </c>
       <c r="M23">
-        <f>Sheet1!M23</f>
         <v>14.999999999999998</v>
       </c>
       <c r="N23">
-        <f>Sheet1!N23</f>
         <v>1241.4953209140724</v>
       </c>
       <c r="O23">
-        <f>Sheet1!O23</f>
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>Sheet1!A24</f>
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
       </c>
       <c r="C24">
-        <f>Sheet1!C24</f>
-        <v>0</v>
+        <v>11.981632679999999</v>
       </c>
       <c r="D24">
-        <f>Sheet1!D24</f>
-        <v>0</v>
+        <v>-13.181818181818182</v>
       </c>
       <c r="E24">
-        <f>Sheet1!E24</f>
-        <v>0</v>
+        <v>1307.0378907317493</v>
       </c>
       <c r="F24">
-        <f>Sheet1!F24</f>
-        <v>0</v>
+        <v>-12.878787878787877</v>
       </c>
       <c r="G24">
-        <f>Sheet1!G24</f>
-        <v>0</v>
+        <v>1252.7629425828798</v>
       </c>
       <c r="H24">
-        <f>Sheet1!H24</f>
-        <v>0</v>
+        <v>19024.110013201633</v>
       </c>
       <c r="I24">
-        <f>Sheet1!I24</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <f>Sheet1!J24</f>
-        <v>0</v>
+        <v>15.996700898233009</v>
       </c>
       <c r="K24">
-        <f>Sheet1!K24</f>
-        <v>0</v>
+        <v>15.996700898233009</v>
       </c>
       <c r="L24">
-        <f>Sheet1!L24</f>
-        <v>0</v>
+        <v>1294.8333098813791</v>
       </c>
       <c r="M24">
-        <f>Sheet1!M24</f>
-        <v>0</v>
+        <v>7.7272727272727275</v>
       </c>
       <c r="N24">
-        <f>Sheet1!N24</f>
-        <v>0</v>
+        <v>1242.7081938396739</v>
       </c>
       <c r="O24">
-        <f>Sheet1!O24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
+        <v>7.7272727272727275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>Sheet1!A25</f>
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>42</v>
       </c>
       <c r="C25">
-        <f>Sheet1!C25</f>
-        <v>0.20319999999999999</v>
+        <v>13.458074640000001</v>
       </c>
       <c r="D25">
-        <f>Sheet1!D25</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="E25">
-        <f>Sheet1!E25</f>
         <v>1246.2893099511575</v>
       </c>
       <c r="F25">
-        <f>Sheet1!F25</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="G25">
-        <f>Sheet1!G25</f>
         <v>1195.4696833375137</v>
       </c>
       <c r="H25">
-        <f>Sheet1!H25</f>
         <v>16336.480118847954</v>
       </c>
       <c r="I25">
-        <f>Sheet1!I25</f>
         <v>1</v>
       </c>
       <c r="J25">
-        <f>Sheet1!J25</f>
         <v>11.730795376588491</v>
       </c>
       <c r="K25">
-        <f>Sheet1!K25</f>
         <v>11.730795376588491</v>
       </c>
       <c r="L25">
-        <f>Sheet1!L25</f>
         <v>1073.4962812291196</v>
       </c>
       <c r="M25">
-        <f>Sheet1!M25</f>
         <v>14.999999999999998</v>
       </c>
       <c r="N25">
-        <f>Sheet1!N25</f>
         <v>1026.9400557288811</v>
       </c>
       <c r="O25">
-        <f>Sheet1!O25</f>
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>Sheet1!A26</f>
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
       <c r="C26">
-        <f>Sheet1!C26</f>
-        <v>0.20319999999999999</v>
+        <v>12.02925984</v>
       </c>
       <c r="D26">
-        <f>Sheet1!D26</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="E26">
-        <f>Sheet1!E26</f>
         <v>1204.6875242675562</v>
       </c>
       <c r="F26">
-        <f>Sheet1!F26</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="G26">
-        <f>Sheet1!G26</f>
         <v>1155.7966927868656</v>
       </c>
       <c r="H26">
-        <f>Sheet1!H26</f>
         <v>16745.947522921681</v>
       </c>
       <c r="I26">
-        <f>Sheet1!I26</f>
         <v>1</v>
       </c>
       <c r="J26">
-        <f>Sheet1!J26</f>
         <v>11.08382078131665</v>
       </c>
       <c r="K26">
-        <f>Sheet1!K26</f>
         <v>11.08382078131665</v>
       </c>
       <c r="L26">
-        <f>Sheet1!L26</f>
         <v>1183.846350683194</v>
       </c>
       <c r="M26">
-        <f>Sheet1!M26</f>
         <v>14.999999999999998</v>
       </c>
       <c r="N26">
-        <f>Sheet1!N26</f>
         <v>1134.2042717181662</v>
       </c>
       <c r="O26">
-        <f>Sheet1!O26</f>
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>Sheet1!A27</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
       </c>
       <c r="C27">
-        <f>Sheet1!C27</f>
-        <v>0.20319999999999999</v>
+        <v>10.763738160000001</v>
       </c>
       <c r="D27">
-        <f>Sheet1!D27</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="E27">
-        <f>Sheet1!E27</f>
         <v>1133.7595009364713</v>
       </c>
       <c r="F27">
-        <f>Sheet1!F27</f>
         <v>-14.999999999999998</v>
       </c>
       <c r="G27">
-        <f>Sheet1!G27</f>
         <v>1086.7320342517114</v>
       </c>
       <c r="H27">
-        <f>Sheet1!H27</f>
         <v>15324.620447760168</v>
       </c>
       <c r="I27">
-        <f>Sheet1!I27</f>
         <v>1</v>
       </c>
       <c r="J27">
-        <f>Sheet1!J27</f>
         <v>13.866556401439492</v>
       </c>
       <c r="K27">
-        <f>Sheet1!K27</f>
         <v>13.866556401439492</v>
       </c>
       <c r="L27">
-        <f>Sheet1!L27</f>
         <v>1055.7157402315393</v>
       </c>
       <c r="M27">
-        <f>Sheet1!M27</f>
         <v>11.363636363636363</v>
       </c>
       <c r="N27">
-        <f>Sheet1!N27</f>
         <v>1010.3873428804375</v>
       </c>
       <c r="O27">
-        <f>Sheet1!O27</f>
         <v>11.363636363636363</v>
       </c>
     </row>
@@ -3679,25 +3402,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
   <dimension ref="B1:AA66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.7109375" customWidth="true"/>
-    <col min="3" max="3" width="21.42578125" customWidth="true"/>
-    <col min="4" max="5" width="18.42578125" customWidth="true"/>
-    <col min="6" max="6" width="13.7109375" bestFit="true" customWidth="true"/>
-    <col min="7" max="10" width="13.7109375" customWidth="true"/>
-    <col min="11" max="11" width="11.5703125" customWidth="true"/>
-    <col min="21" max="21" width="37.85546875" customWidth="true"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="21" max="21" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
       <c r="F1" s="16" t="s">
         <v>37</v>
       </c>
@@ -3705,12 +3428,12 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" ht="39" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" ht="39" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>Sheet1!$B$1</f>
         <v>'tyre'</v>
@@ -3761,7 +3484,7 @@
         <v>22</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
@@ -3808,7 +3531,7 @@
         <v>1.4750000000000001</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
@@ -3851,7 +3574,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="2"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>Sheet2!B2</f>
         <v>01_Hoosier_16x7.5-10_R20_7Rim.tir</v>
@@ -3894,7 +3617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>Sheet2!B3</f>
         <v>02_Hoosier_16x7.5-10_R20_8Rim.tir</v>
@@ -3940,7 +3663,7 @@
         <v>28</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>Sheet2!B4</f>
         <v>03_Hoosier_16x6.0-10_R20_6Rim.tir</v>
@@ -3995,7 +3718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f>Sheet2!B5</f>
         <v>04_Hoosier_16x6.0-10_R20_7Rim.tir</v>
@@ -4038,7 +3761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>Sheet2!B6</f>
         <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
@@ -4081,7 +3804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>Sheet2!B7</f>
         <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
@@ -4124,7 +3847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>Sheet2!B8</f>
         <v>07_Goodyear_18.0x6.5-10_D0571_6Rim.tir</v>
@@ -4167,7 +3890,7 @@
         <v>18</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>Sheet2!B9</f>
         <v>08_Goodyear_18.0x6.5-10_D0571_7Rim.tir</v>
@@ -4210,7 +3933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>Sheet2!B10</f>
         <v>09_MRF_18x6-10_ZTD1_6Rim.tir</v>
@@ -4253,7 +3976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>Sheet2!B11</f>
         <v>10_MRF_18x6-10_ZTD1_7Rim.tir</v>
@@ -4296,7 +4019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>Sheet2!B12</f>
         <v>11_Hoosier_20.5x7-13_R20_7Rim.tir</v>
@@ -4339,7 +4062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>Sheet2!B13</f>
         <v>12_Hoosier_20.5x7-13_R20_8Rim.tir</v>
@@ -4379,7 +4102,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>Sheet2!B14</f>
         <v>13_Goodyear_20.0x7-13_D2704_7Rim.tir</v>
@@ -4419,7 +4142,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>Sheet2!B15</f>
         <v>14_Goodyear_20.0x7-13_D2704_8Rim.tir</v>
@@ -4459,7 +4182,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>Sheet2!B16</f>
         <v>15_Continental_205x470R-13_FS43329_7Rim.tir</v>
@@ -4499,7 +4222,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>Sheet2!B17</f>
         <v>16_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
@@ -4539,7 +4262,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>Sheet2!B18</f>
         <v>17_Hoosier_16.0x6.0-10_LCO_7Rim.tir</v>
@@ -4579,7 +4302,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>Sheet2!B19</f>
         <v>18_Hoosier_16.0x7.5-10_LCO_8Rim.tir</v>
@@ -4619,7 +4342,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>Sheet2!B20</f>
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
@@ -4659,7 +4382,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>Sheet2!B21</f>
         <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
@@ -4699,10 +4422,10 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
-      <c r="B27">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
         <f>Sheet2!B22</f>
-        <v>0</v>
+        <v>21_Avon_7.0x16.0-10_FS_8Rim.tir</v>
       </c>
       <c r="C27" s="9" t="e">
         <f>Sheet1!#REF!</f>
@@ -4739,10 +4462,10 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.25">
-      <c r="B28">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
         <f>Sheet2!B23</f>
-        <v>0</v>
+        <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
       </c>
       <c r="C28" s="9" t="e">
         <f>Sheet1!#REF!</f>
@@ -4779,10 +4502,10 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" x14ac:dyDescent="0.25">
-      <c r="B29">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
         <f>Sheet2!B24</f>
-        <v>0</v>
+        <v>23_Avon_8.2x20.0-13_FS_9Rim.tir</v>
       </c>
       <c r="C29" s="9" t="e">
         <f>Sheet1!#REF!</f>
@@ -4819,7 +4542,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f>Sheet2!B25</f>
         <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
@@ -4859,7 +4582,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>Sheet2!B26</f>
         <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
@@ -4899,7 +4622,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>Sheet2!B27</f>
         <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
@@ -4939,7 +4662,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>Sheet2!B28</f>
         <v>0</v>
@@ -4979,12 +4702,12 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="36" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="37" ht="39" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" ht="39" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>Sheet1!$B$1</f>
         <v>'tyre'</v>
@@ -5035,7 +4758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="38" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>23</v>
       </c>
@@ -5096,7 +4819,7 @@
         <v>1.4500000000000002</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="39" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>24</v>
       </c>
@@ -5161,7 +4884,7 @@
         <v>40</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="40" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>B7</f>
         <v>01_Hoosier_16x7.5-10_R20_7Rim.tir</v>
@@ -5208,7 +4931,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="41" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f t="shared" ref="B41:B66" si="4">B8</f>
         <v>02_Hoosier_16x7.5-10_R20_8Rim.tir</v>
@@ -5255,7 +4978,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="42" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f t="shared" si="4"/>
         <v>03_Hoosier_16x6.0-10_R20_6Rim.tir</v>
@@ -5302,7 +5025,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="43" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f t="shared" si="4"/>
         <v>04_Hoosier_16x6.0-10_R20_7Rim.tir</v>
@@ -5349,7 +5072,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="44" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f t="shared" si="4"/>
         <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
@@ -5396,7 +5119,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f t="shared" si="4"/>
         <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
@@ -5443,7 +5166,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="46" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f t="shared" si="4"/>
         <v>07_Goodyear_18.0x6.5-10_D0571_6Rim.tir</v>
@@ -5490,7 +5213,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="47" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f t="shared" si="4"/>
         <v>08_Goodyear_18.0x6.5-10_D0571_7Rim.tir</v>
@@ -5537,7 +5260,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="48" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f t="shared" si="4"/>
         <v>09_MRF_18x6-10_ZTD1_6Rim.tir</v>
@@ -5584,7 +5307,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="49" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f t="shared" si="4"/>
         <v>10_MRF_18x6-10_ZTD1_7Rim.tir</v>
@@ -5631,7 +5354,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="50" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f t="shared" si="4"/>
         <v>11_Hoosier_20.5x7-13_R20_7Rim.tir</v>
@@ -5678,7 +5401,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="51" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f t="shared" si="4"/>
         <v>12_Hoosier_20.5x7-13_R20_8Rim.tir</v>
@@ -5725,7 +5448,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="52" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f t="shared" si="4"/>
         <v>13_Goodyear_20.0x7-13_D2704_7Rim.tir</v>
@@ -5772,7 +5495,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="53" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f t="shared" si="4"/>
         <v>14_Goodyear_20.0x7-13_D2704_8Rim.tir</v>
@@ -5819,7 +5542,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="54" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f t="shared" si="4"/>
         <v>15_Continental_205x470R-13_FS43329_7Rim.tir</v>
@@ -5855,7 +5578,7 @@
       </c>
       <c r="L54" s="9">
         <f>Sheet1!G22</f>
-        <v>0</v>
+        <v>1202.8817765036304</v>
       </c>
       <c r="Q54" s="18" t="e">
         <f t="shared" si="10"/>
@@ -5866,7 +5589,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="55" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f t="shared" si="4"/>
         <v>16_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
@@ -5913,7 +5636,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="56" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f t="shared" si="4"/>
         <v>17_Hoosier_16.0x6.0-10_LCO_7Rim.tir</v>
@@ -5949,7 +5672,7 @@
       </c>
       <c r="L56" s="9">
         <f>Sheet1!G24</f>
-        <v>0</v>
+        <v>1252.7629425828798</v>
       </c>
       <c r="Q56" s="18" t="e">
         <f t="shared" si="10"/>
@@ -5960,7 +5683,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="57" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f t="shared" si="4"/>
         <v>18_Hoosier_16.0x7.5-10_LCO_8Rim.tir</v>
@@ -6007,7 +5730,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="58" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f t="shared" si="4"/>
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
@@ -6054,7 +5777,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="59" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
         <f t="shared" si="4"/>
         <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
@@ -6101,10 +5824,10 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="60" x14ac:dyDescent="0.25">
-      <c r="B60">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B60" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>21_Avon_7.0x16.0-10_FS_8Rim.tir</v>
       </c>
       <c r="C60" s="18" t="e">
         <f t="shared" si="5"/>
@@ -6148,10 +5871,10 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="61" x14ac:dyDescent="0.25">
-      <c r="B61">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B61" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
       </c>
       <c r="C61" s="18" t="e">
         <f t="shared" si="5"/>
@@ -6195,10 +5918,10 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="62" x14ac:dyDescent="0.25">
-      <c r="B62">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B62" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>23_Avon_8.2x20.0-13_FS_9Rim.tir</v>
       </c>
       <c r="C62" s="18" t="e">
         <f t="shared" si="5"/>
@@ -6242,7 +5965,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="63" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f t="shared" si="4"/>
         <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
@@ -6289,7 +6012,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="64" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f t="shared" si="4"/>
         <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
@@ -6336,7 +6059,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="65" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
         <f t="shared" si="4"/>
         <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
@@ -6383,7 +6106,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="66" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6438,7 +6161,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6450,7 +6173,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6462,7 +6185,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6474,7 +6197,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6486,7 +6209,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6498,7 +6221,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6510,7 +6233,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6522,7 +6245,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6534,7 +6257,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038484"/>
+        <color theme="9" tint="0.79995117038483843"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6544,19 +6267,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9038B9-1403-4B22-9A5D-BC5487C92A60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9038B9-1403-4B22-9A5D-BC5487C92A60}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.28515625" customWidth="true"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -6564,61 +6287,61 @@
         <v>41</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="e">
-        <f ca="true">xlookup(A2,Sheet3!B40:B66, Sheet3!R40:R66)</f>
+        <f ca="1">xlookup(A2,Sheet3!B40:B66, Sheet3!R40:R66)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Minor changes. Dw about it
</commit_message>
<xml_diff>
--- a/model_outputs/tyre_ranking.xlsx
+++ b/model_outputs/tyre_ranking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\292255A\Documents\GitHub\cmt_tyre_toolbox_new\model_outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5C500E-72D7-4CBD-86BE-F5E26EFD6C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BD6E60-6C76-4CDC-A4D7-3A6A6E0F75E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="70">
   <si>
     <t>'SA_at_FY_max'</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>23_Avon_8.2x20.0-13_FS_9Rim.tir</t>
+  </si>
+  <si>
+    <t>29_Hoosier_16.0x6.0-10_LCO_6Rim.tir</t>
   </si>
 </sst>
 </file>
@@ -766,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,6 +2078,47 @@
       </c>
       <c r="O27">
         <v>11.363636363636363</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30">
+        <v>5.1323934799999993</v>
+      </c>
+      <c r="D30">
+        <v>-12.272727272727272</v>
+      </c>
+      <c r="E30">
+        <v>1405.4454568506501</v>
+      </c>
+      <c r="F30">
+        <v>-12.272727272727272</v>
+      </c>
+      <c r="G30">
+        <v>1353.4044916495345</v>
+      </c>
+      <c r="H30">
+        <v>19958.48151666945</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>22.83479006064082</v>
+      </c>
+      <c r="K30">
+        <v>22.83479006064082</v>
+      </c>
+      <c r="L30">
+        <v>1243.88559213399</v>
+      </c>
+      <c r="N30">
+        <v>1191.4505197219842</v>
       </c>
     </row>
   </sheetData>
@@ -5954,7 +5998,7 @@
       </c>
       <c r="L62" s="9">
         <f>Sheet1!G30</f>
-        <v>0</v>
+        <v>1353.4044916495345</v>
       </c>
       <c r="Q62" s="18" t="e">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
Included driver weight.. Becuase I originally forgot
</commit_message>
<xml_diff>
--- a/model_outputs/tyre_ranking.xlsx
+++ b/model_outputs/tyre_ranking.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BD6E60-6C76-4CDC-A4D7-3A6A6E0F75E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="218" uniqueCount="70">
   <si>
     <t>'SA_at_FY_max'</t>
   </si>
@@ -243,11 +243,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -384,57 +384,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +455,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -604,7 +606,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -628,9 +630,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -654,7 +656,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -689,7 +691,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -707,7 +709,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -732,7 +734,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -768,56 +770,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5360D38-CECE-47B1-AE8F-8AD4BEDE1BBF}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="true" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" customWidth="1"/>
-    <col min="16" max="22" width="12.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
-    <col min="25" max="33" width="11.5703125" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" customWidth="1"/>
-    <col min="35" max="36" width="11.5703125" customWidth="1"/>
-    <col min="37" max="37" width="10.5703125" customWidth="1"/>
-    <col min="38" max="38" width="9.5703125" customWidth="1"/>
-    <col min="39" max="55" width="11.5703125" customWidth="1"/>
-    <col min="56" max="56" width="10.5703125" customWidth="1"/>
-    <col min="57" max="77" width="11.5703125" customWidth="1"/>
-    <col min="78" max="78" width="10.5703125" customWidth="1"/>
-    <col min="79" max="90" width="11.5703125" customWidth="1"/>
-    <col min="91" max="91" width="10.5703125" customWidth="1"/>
-    <col min="92" max="98" width="11.5703125" customWidth="1"/>
-    <col min="99" max="103" width="12.28515625" customWidth="1"/>
-    <col min="104" max="104" width="11.28515625" customWidth="1"/>
-    <col min="105" max="105" width="12.28515625" customWidth="1"/>
-    <col min="106" max="106" width="10.28515625" customWidth="1"/>
-    <col min="107" max="107" width="10.5703125" customWidth="1"/>
-    <col min="108" max="110" width="2.140625" customWidth="1"/>
-    <col min="111" max="111" width="11.5703125" customWidth="1"/>
-    <col min="113" max="113" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="40.875" customWidth="true"/>
+    <col min="3" max="3" width="14.5" customWidth="true"/>
+    <col min="4" max="4" width="15" customWidth="true"/>
+    <col min="5" max="5" width="22.875" customWidth="true"/>
+    <col min="6" max="6" width="17" customWidth="true"/>
+    <col min="7" max="7" width="15.375" customWidth="true"/>
+    <col min="8" max="8" width="13.125" customWidth="true"/>
+    <col min="9" max="9" width="13.375" customWidth="true"/>
+    <col min="10" max="10" width="11.625" customWidth="true"/>
+    <col min="11" max="11" width="14.625" customWidth="true"/>
+    <col min="12" max="12" width="15" customWidth="true"/>
+    <col min="13" max="13" width="14.75" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="17" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="23.125" customWidth="true"/>
+    <col min="16" max="22" width="12.28515625" customWidth="true"/>
+    <col min="23" max="23" width="11.28515625" customWidth="true"/>
+    <col min="24" max="24" width="12.28515625" customWidth="true"/>
+    <col min="25" max="33" width="11.5703125" customWidth="true"/>
+    <col min="34" max="34" width="10.5703125" customWidth="true"/>
+    <col min="35" max="36" width="11.5703125" customWidth="true"/>
+    <col min="37" max="37" width="10.5703125" customWidth="true"/>
+    <col min="38" max="38" width="9.5703125" customWidth="true"/>
+    <col min="39" max="55" width="11.5703125" customWidth="true"/>
+    <col min="56" max="56" width="10.5703125" customWidth="true"/>
+    <col min="57" max="77" width="11.5703125" customWidth="true"/>
+    <col min="78" max="78" width="10.5703125" customWidth="true"/>
+    <col min="79" max="90" width="11.5703125" customWidth="true"/>
+    <col min="91" max="91" width="10.5703125" customWidth="true"/>
+    <col min="92" max="98" width="11.5703125" customWidth="true"/>
+    <col min="99" max="103" width="12.28515625" customWidth="true"/>
+    <col min="104" max="104" width="11.28515625" customWidth="true"/>
+    <col min="105" max="105" width="12.28515625" customWidth="true"/>
+    <col min="106" max="106" width="10.28515625" customWidth="true"/>
+    <col min="107" max="107" width="10.5703125" customWidth="true"/>
+    <col min="108" max="110" width="2.140625" customWidth="true"/>
+    <col min="111" max="111" width="11.5703125" customWidth="true"/>
+    <col min="113" max="113" width="11.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -864,7 +866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -911,7 +913,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -958,7 +960,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1005,7 +1007,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>10.757575757575756</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1140,7 +1142,7 @@
         <v>1199.7725693945349</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1187,7 +1189,7 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1234,7 +1236,7 @@
         <v>6.2121212121212119</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1281,7 +1283,7 @@
         <v>4.3939393939393936</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1328,7 +1330,7 @@
         <v>8.9393939393939377</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1375,7 +1377,7 @@
         <v>8.0303030303030294</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1422,7 +1424,7 @@
         <v>7.7272727272727275</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1469,7 +1471,7 @@
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1516,7 +1518,7 @@
         <v>7.1212121212121202</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1563,7 +1565,7 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1610,7 +1612,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1704,7 +1706,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1751,7 +1753,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1798,7 +1800,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1892,7 +1894,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1939,7 +1941,7 @@
         <v>7.7272727272727275</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1986,7 +1988,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2033,7 +2035,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2080,46 +2082,48 @@
         <v>11.363636363636363</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="0">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="0">
         <v>5.1323934799999993</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="0">
         <v>-12.272727272727272</v>
       </c>
-      <c r="E30">
-        <v>1405.4454568506501</v>
-      </c>
-      <c r="F30">
+      <c r="E30" s="0">
+        <v>1903.8369668870264</v>
+      </c>
+      <c r="F30" s="0">
         <v>-12.272727272727272</v>
       </c>
-      <c r="G30">
-        <v>1353.4044916495345</v>
-      </c>
-      <c r="H30">
-        <v>19958.48151666945</v>
-      </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <v>22.83479006064082</v>
-      </c>
-      <c r="K30">
-        <v>22.83479006064082</v>
-      </c>
-      <c r="L30">
-        <v>1243.88559213399</v>
-      </c>
-      <c r="N30">
-        <v>1191.4505197219842</v>
-      </c>
+      <c r="G30" s="0">
+        <v>1858.8878181756145</v>
+      </c>
+      <c r="H30" s="0">
+        <v>25513.93773219192</v>
+      </c>
+      <c r="I30" s="0">
+        <v>1</v>
+      </c>
+      <c r="J30" s="0">
+        <v>39.92443937042701</v>
+      </c>
+      <c r="K30" s="0">
+        <v>39.92443937042701</v>
+      </c>
+      <c r="L30" s="0">
+        <v>1784.7845514473252</v>
+      </c>
+      <c r="M30" s="0"/>
+      <c r="N30" s="0">
+        <v>1732.7538489002443</v>
+      </c>
+      <c r="O30" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2128,56 +2132,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9898B6A-1213-468B-847F-2F72FED041C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9898B6A-1213-468B-847F-2F72FED041C5}">
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" customWidth="1"/>
-    <col min="16" max="22" width="12.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
-    <col min="25" max="33" width="11.5703125" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" customWidth="1"/>
-    <col min="35" max="36" width="11.5703125" customWidth="1"/>
-    <col min="37" max="37" width="10.5703125" customWidth="1"/>
-    <col min="38" max="38" width="9.5703125" customWidth="1"/>
-    <col min="39" max="55" width="11.5703125" customWidth="1"/>
-    <col min="56" max="56" width="10.5703125" customWidth="1"/>
-    <col min="57" max="77" width="11.5703125" customWidth="1"/>
-    <col min="78" max="78" width="10.5703125" customWidth="1"/>
-    <col min="79" max="90" width="11.5703125" customWidth="1"/>
-    <col min="91" max="91" width="10.5703125" customWidth="1"/>
-    <col min="92" max="98" width="11.5703125" customWidth="1"/>
-    <col min="99" max="103" width="12.28515625" customWidth="1"/>
-    <col min="104" max="104" width="11.28515625" customWidth="1"/>
-    <col min="105" max="105" width="12.28515625" customWidth="1"/>
-    <col min="106" max="106" width="10.28515625" customWidth="1"/>
-    <col min="107" max="107" width="10.5703125" customWidth="1"/>
-    <col min="108" max="110" width="2.140625" customWidth="1"/>
-    <col min="111" max="111" width="11.5703125" customWidth="1"/>
-    <col min="113" max="113" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="40.85546875" customWidth="true"/>
+    <col min="3" max="3" width="14.42578125" customWidth="true"/>
+    <col min="4" max="4" width="15" customWidth="true"/>
+    <col min="5" max="5" width="22.85546875" customWidth="true"/>
+    <col min="6" max="6" width="17" customWidth="true"/>
+    <col min="7" max="7" width="15.42578125" customWidth="true"/>
+    <col min="8" max="8" width="13.140625" customWidth="true"/>
+    <col min="9" max="9" width="13.42578125" customWidth="true"/>
+    <col min="10" max="10" width="11.5703125" customWidth="true"/>
+    <col min="11" max="11" width="14.5703125" customWidth="true"/>
+    <col min="12" max="12" width="15" customWidth="true"/>
+    <col min="13" max="13" width="14.7109375" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="17" bestFit="true" customWidth="true"/>
+    <col min="15" max="15" width="23.140625" customWidth="true"/>
+    <col min="16" max="22" width="12.28515625" customWidth="true"/>
+    <col min="23" max="23" width="11.28515625" customWidth="true"/>
+    <col min="24" max="24" width="12.28515625" customWidth="true"/>
+    <col min="25" max="33" width="11.5703125" customWidth="true"/>
+    <col min="34" max="34" width="10.5703125" customWidth="true"/>
+    <col min="35" max="36" width="11.5703125" customWidth="true"/>
+    <col min="37" max="37" width="10.5703125" customWidth="true"/>
+    <col min="38" max="38" width="9.5703125" customWidth="true"/>
+    <col min="39" max="55" width="11.5703125" customWidth="true"/>
+    <col min="56" max="56" width="10.5703125" customWidth="true"/>
+    <col min="57" max="77" width="11.5703125" customWidth="true"/>
+    <col min="78" max="78" width="10.5703125" customWidth="true"/>
+    <col min="79" max="90" width="11.5703125" customWidth="true"/>
+    <col min="91" max="91" width="10.5703125" customWidth="true"/>
+    <col min="92" max="98" width="11.5703125" customWidth="true"/>
+    <col min="99" max="103" width="12.28515625" customWidth="true"/>
+    <col min="104" max="104" width="11.28515625" customWidth="true"/>
+    <col min="105" max="105" width="12.28515625" customWidth="true"/>
+    <col min="106" max="106" width="10.28515625" customWidth="true"/>
+    <col min="107" max="107" width="10.5703125" customWidth="true"/>
+    <col min="108" max="110" width="2.140625" customWidth="true"/>
+    <col min="111" max="111" width="11.5703125" customWidth="true"/>
+    <col min="113" max="113" width="11.5703125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2224,7 +2228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2271,7 +2275,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2318,7 +2322,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2365,7 +2369,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2412,7 +2416,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2459,7 +2463,7 @@
         <v>10.757575757575756</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2500,7 +2504,7 @@
         <v>1199.7725693945349</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2547,7 +2551,7 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2594,7 +2598,7 @@
         <v>6.2121212121212119</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2641,7 +2645,7 @@
         <v>4.3939393939393936</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2688,7 +2692,7 @@
         <v>8.9393939393939377</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2735,7 +2739,7 @@
         <v>8.0303030303030294</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2782,7 +2786,7 @@
         <v>7.7272727272727275</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>8.3333333333333321</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2876,7 +2880,7 @@
         <v>7.1212121212121202</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2923,7 +2927,7 @@
         <v>5.9090909090909092</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2970,7 +2974,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3017,7 +3021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3064,7 +3068,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3111,7 +3115,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3158,7 +3162,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3205,7 +3209,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3252,7 +3256,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3299,7 +3303,7 @@
         <v>7.7272727272727275</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3346,7 +3350,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3393,7 +3397,7 @@
         <v>14.999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3446,25 +3450,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6D7A46-FEE7-499E-BC4A-8F28CEEB05E7}">
   <dimension ref="B1:AA66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="true"/>
+    <col min="3" max="3" width="21.42578125" customWidth="true"/>
+    <col min="4" max="5" width="18.42578125" customWidth="true"/>
+    <col min="6" max="6" width="13.7109375" bestFit="true" customWidth="true"/>
+    <col min="7" max="10" width="13.7109375" customWidth="true"/>
+    <col min="11" max="11" width="11.5703125" customWidth="true"/>
+    <col min="21" max="21" width="37.85546875" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="F1" s="16" t="s">
         <v>37</v>
       </c>
@@ -3472,12 +3476,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:27" ht="39" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" ht="39" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>Sheet1!$B$1</f>
         <v>'tyre'</v>
@@ -3528,7 +3532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
@@ -3575,7 +3579,7 @@
         <v>1.4750000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
@@ -3618,7 +3622,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>Sheet2!B2</f>
         <v>01_Hoosier_16x7.5-10_R20_7Rim.tir</v>
@@ -3661,7 +3665,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>Sheet2!B3</f>
         <v>02_Hoosier_16x7.5-10_R20_8Rim.tir</v>
@@ -3707,7 +3711,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>Sheet2!B4</f>
         <v>03_Hoosier_16x6.0-10_R20_6Rim.tir</v>
@@ -3762,7 +3766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f>Sheet2!B5</f>
         <v>04_Hoosier_16x6.0-10_R20_7Rim.tir</v>
@@ -3805,7 +3809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>Sheet2!B6</f>
         <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
@@ -3848,7 +3852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>Sheet2!B7</f>
         <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
@@ -3891,7 +3895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>Sheet2!B8</f>
         <v>07_Goodyear_18.0x6.5-10_D0571_6Rim.tir</v>
@@ -3934,7 +3938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>Sheet2!B9</f>
         <v>08_Goodyear_18.0x6.5-10_D0571_7Rim.tir</v>
@@ -3977,7 +3981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="15" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>Sheet2!B10</f>
         <v>09_MRF_18x6-10_ZTD1_6Rim.tir</v>
@@ -4020,7 +4024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="16" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>Sheet2!B11</f>
         <v>10_MRF_18x6-10_ZTD1_7Rim.tir</v>
@@ -4063,7 +4067,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="17" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f>Sheet2!B12</f>
         <v>11_Hoosier_20.5x7-13_R20_7Rim.tir</v>
@@ -4106,7 +4110,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="18" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>Sheet2!B13</f>
         <v>12_Hoosier_20.5x7-13_R20_8Rim.tir</v>
@@ -4146,7 +4150,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="19" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>Sheet2!B14</f>
         <v>13_Goodyear_20.0x7-13_D2704_7Rim.tir</v>
@@ -4186,7 +4190,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="20" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>Sheet2!B15</f>
         <v>14_Goodyear_20.0x7-13_D2704_8Rim.tir</v>
@@ -4226,7 +4230,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="21" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>Sheet2!B16</f>
         <v>15_Continental_205x470R-13_FS43329_7Rim.tir</v>
@@ -4266,7 +4270,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="22" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>Sheet2!B17</f>
         <v>16_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
@@ -4306,7 +4310,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="23" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>Sheet2!B18</f>
         <v>17_Hoosier_16.0x6.0-10_LCO_7Rim.tir</v>
@@ -4346,7 +4350,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="24" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>Sheet2!B19</f>
         <v>18_Hoosier_16.0x7.5-10_LCO_8Rim.tir</v>
@@ -4386,7 +4390,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="25" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>Sheet2!B20</f>
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
@@ -4426,7 +4430,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="26" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>Sheet2!B21</f>
         <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
@@ -4466,7 +4470,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="27" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>Sheet2!B22</f>
         <v>21_Avon_7.0x16.0-10_FS_8Rim.tir</v>
@@ -4506,7 +4510,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="28" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>Sheet2!B23</f>
         <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
@@ -4546,7 +4550,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="29" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
         <f>Sheet2!B24</f>
         <v>23_Avon_8.2x20.0-13_FS_9Rim.tir</v>
@@ -4586,7 +4590,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="30" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f>Sheet2!B25</f>
         <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
@@ -4626,7 +4630,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="31" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>Sheet2!B26</f>
         <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
@@ -4666,7 +4670,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="32" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>Sheet2!B27</f>
         <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
@@ -4706,7 +4710,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="33" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>Sheet2!B28</f>
         <v>0</v>
@@ -4746,12 +4750,12 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="36" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:18" ht="39" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="37" ht="39" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>Sheet1!$B$1</f>
         <v>'tyre'</v>
@@ -4802,7 +4806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="38" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>23</v>
       </c>
@@ -4863,7 +4867,7 @@
         <v>1.4500000000000002</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="39" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>24</v>
       </c>
@@ -4928,7 +4932,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="40" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>B7</f>
         <v>01_Hoosier_16x7.5-10_R20_7Rim.tir</v>
@@ -4975,7 +4979,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="41" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f t="shared" ref="B41:B66" si="4">B8</f>
         <v>02_Hoosier_16x7.5-10_R20_8Rim.tir</v>
@@ -5022,7 +5026,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="42" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f t="shared" si="4"/>
         <v>03_Hoosier_16x6.0-10_R20_6Rim.tir</v>
@@ -5069,7 +5073,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="43" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f t="shared" si="4"/>
         <v>04_Hoosier_16x6.0-10_R20_7Rim.tir</v>
@@ -5116,7 +5120,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="44" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f t="shared" si="4"/>
         <v>05_Hoosier_18x6.0-10_R20_6Rim.tir</v>
@@ -5163,7 +5167,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="45" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f t="shared" si="4"/>
         <v>06_Hoosier_18x6.0-10_R20_7Rim.tir</v>
@@ -5210,7 +5214,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="46" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f t="shared" si="4"/>
         <v>07_Goodyear_18.0x6.5-10_D0571_6Rim.tir</v>
@@ -5257,7 +5261,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="47" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f t="shared" si="4"/>
         <v>08_Goodyear_18.0x6.5-10_D0571_7Rim.tir</v>
@@ -5304,7 +5308,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="48" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f t="shared" si="4"/>
         <v>09_MRF_18x6-10_ZTD1_6Rim.tir</v>
@@ -5351,7 +5355,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="49" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f t="shared" si="4"/>
         <v>10_MRF_18x6-10_ZTD1_7Rim.tir</v>
@@ -5398,7 +5402,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="50" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f t="shared" si="4"/>
         <v>11_Hoosier_20.5x7-13_R20_7Rim.tir</v>
@@ -5445,7 +5449,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="51" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f t="shared" si="4"/>
         <v>12_Hoosier_20.5x7-13_R20_8Rim.tir</v>
@@ -5492,7 +5496,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="52" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f t="shared" si="4"/>
         <v>13_Goodyear_20.0x7-13_D2704_7Rim.tir</v>
@@ -5539,7 +5543,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="53" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f t="shared" si="4"/>
         <v>14_Goodyear_20.0x7-13_D2704_8Rim.tir</v>
@@ -5586,7 +5590,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="54" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f t="shared" si="4"/>
         <v>15_Continental_205x470R-13_FS43329_7Rim.tir</v>
@@ -5633,7 +5637,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="55" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f t="shared" si="4"/>
         <v>16_Hoosier_16.0x6.0-10_LCO_6Rim.tir</v>
@@ -5680,7 +5684,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="56" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f t="shared" si="4"/>
         <v>17_Hoosier_16.0x6.0-10_LCO_7Rim.tir</v>
@@ -5727,7 +5731,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="57" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f t="shared" si="4"/>
         <v>18_Hoosier_16.0x7.5-10_LCO_8Rim.tir</v>
@@ -5774,7 +5778,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="58" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f t="shared" si="4"/>
         <v>19_Hoosier_16.0x7.5-10_LCO_7Rim.tir</v>
@@ -5821,7 +5825,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="59" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
         <f t="shared" si="4"/>
         <v>20_Avon_7.0x16.0-10_FS_7Rim.tir</v>
@@ -5868,7 +5872,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="60" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
         <f t="shared" si="4"/>
         <v>21_Avon_7.0x16.0-10_FS_8Rim.tir</v>
@@ -5915,7 +5919,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="61" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
         <f t="shared" si="4"/>
         <v>22_Avon_8.2x20.0-13_FS_8Rim.tir</v>
@@ -5962,7 +5966,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="62" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
         <f t="shared" si="4"/>
         <v>23_Avon_8.2x20.0-13_FS_9Rim.tir</v>
@@ -6009,7 +6013,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="63" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f t="shared" si="4"/>
         <v>24_Avon_7.2x20.0-13_FS_7Rim.tir</v>
@@ -6056,7 +6060,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="64" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f t="shared" si="4"/>
         <v>25_Avon_7.2x20.0-13_FS_8Rim.tir</v>
@@ -6103,7 +6107,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="65" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
         <f t="shared" si="4"/>
         <v>26_Avon_6.2x20.0-13_FS_6Rim.tir</v>
@@ -6150,7 +6154,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="66" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -6205,7 +6209,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6217,7 +6221,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6229,7 +6233,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6241,7 +6245,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6253,7 +6257,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6265,7 +6269,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6277,7 +6281,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6289,7 +6293,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6301,7 +6305,7 @@
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color theme="2"/>
-        <color theme="9" tint="0.79995117038483843"/>
+        <color theme="9" tint="0.79995117038484"/>
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
@@ -6311,19 +6315,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9038B9-1403-4B22-9A5D-BC5487C92A60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9038B9-1403-4B22-9A5D-BC5487C92A60}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -6331,61 +6335,61 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="e">
-        <f ca="1">xlookup(A2,Sheet3!B40:B66, Sheet3!R40:R66)</f>
+        <f ca="true">xlookup(A2,Sheet3!B40:B66, Sheet3!R40:R66)</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>

</xml_diff>